<commit_message>
feat: Implémentation stratégie ESG Long-Only + rapport complet
- Ajout politique exclusion ESG (32 titres exclus)
- Filtrage tabac, armes, fossiles, jeux, alcool dans config.py
- Application filtre ESG dans main.py (395 -> 363 titres)
- Amélioration affichage portefeuille (4 décimales)
- Export CSV portefeuille actuel (ticker + weights)
- Ajout rapport_strategie.md complet
- Mise à jour outputs avec stratégie ESG
- Performance finale: CAGR 24.36%, Sharpe 3.22, Vol 6.94%
</commit_message>
<xml_diff>
--- a/outputs/backtest_results.xlsx
+++ b/outputs/backtest_results.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26.62%</t>
+          <t>24.36%</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7.89%</t>
+          <t>6.94%</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3.12</t>
+          <t>3.22</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5.32</t>
+          <t>5.40</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-5.13%</t>
+          <t>-3.80%</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>944.72%</t>
+          <t>779.36%</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-1.81%</t>
+          <t>-1.42%</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>-3.21%</t>
+          <t>-2.95%</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>39.64%</t>
+          <t>40.79%</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2.3781%</t>
+          <t>2.4473%</t>
         </is>
       </c>
     </row>
@@ -623,10 +623,10 @@
         <v>42398</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01362097970305694</v>
+        <v>0.006290996569597647</v>
       </c>
       <c r="C2" t="n">
-        <v>1.013620979703057</v>
+        <v>1.006290996569598</v>
       </c>
       <c r="D2" t="n">
         <v>0.5</v>
@@ -640,16 +640,16 @@
         <v>42429</v>
       </c>
       <c r="B3" t="n">
-        <v>0.002061345377916831</v>
+        <v>0.008320802291742434</v>
       </c>
       <c r="C3" t="n">
-        <v>1.015710402624527</v>
+        <v>1.014664145000014</v>
       </c>
       <c r="D3" t="n">
-        <v>0.28</v>
+        <v>0.36</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00014</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="4">
@@ -657,16 +657,16 @@
         <v>42460</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0407688220479662</v>
+        <v>0.04417395839585556</v>
       </c>
       <c r="C4" t="n">
-        <v>1.057119719281395</v>
+        <v>1.059485876727011</v>
       </c>
       <c r="D4" t="n">
-        <v>0.28</v>
+        <v>0.36</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00014</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="5">
@@ -674,16 +674,16 @@
         <v>42489</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.004327796459335166</v>
+        <v>-0.001662187977838909</v>
       </c>
       <c r="C5" t="n">
-        <v>1.052544720303195</v>
+        <v>1.057724812040025</v>
       </c>
       <c r="D5" t="n">
-        <v>0.36</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00018</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="6">
@@ -691,16 +691,16 @@
         <v>42521</v>
       </c>
       <c r="B6" t="n">
-        <v>0.01985739189078521</v>
+        <v>0.01536474409835926</v>
       </c>
       <c r="C6" t="n">
-        <v>1.073445513296833</v>
+        <v>1.073976483103505</v>
       </c>
       <c r="D6" t="n">
-        <v>0.28</v>
+        <v>0.3200000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00014</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="7">
@@ -708,16 +708,16 @@
         <v>42551</v>
       </c>
       <c r="B7" t="n">
-        <v>0.02644721234083387</v>
+        <v>0.0271652551712853</v>
       </c>
       <c r="C7" t="n">
-        <v>1.101835154723309</v>
+        <v>1.103151328314972</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4800000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0002400000000000001</v>
+        <v>0.00026</v>
       </c>
     </row>
     <row r="8">
@@ -725,16 +725,16 @@
         <v>42580</v>
       </c>
       <c r="B8" t="n">
-        <v>0.03313315921756058</v>
+        <v>0.0277168627445631</v>
       </c>
       <c r="C8" t="n">
-        <v>1.138342434336262</v>
+        <v>1.13372722226836</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3200000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="E8" t="n">
-        <v>0.00016</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="9">
@@ -742,16 +742,16 @@
         <v>42613</v>
       </c>
       <c r="B9" t="n">
-        <v>0.008750933227817866</v>
+        <v>0.01116957787276499</v>
       </c>
       <c r="C9" t="n">
-        <v>1.148303992969531</v>
+        <v>1.14639047676396</v>
       </c>
       <c r="D9" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00018</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="10">
@@ -759,16 +759,16 @@
         <v>42643</v>
       </c>
       <c r="B10" t="n">
-        <v>0.006246642787642528</v>
+        <v>0.00527244810987141</v>
       </c>
       <c r="C10" t="n">
-        <v>1.155477037825235</v>
+        <v>1.152434761066349</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2500000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000125</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="11">
@@ -776,10 +776,10 @@
         <v>42674</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.01173514771326831</v>
+        <v>-0.008079432916362954</v>
       </c>
       <c r="C11" t="n">
-        <v>1.141917344107066</v>
+        <v>1.143123741723829</v>
       </c>
       <c r="D11" t="n">
         <v>0.6400000000000001</v>
@@ -793,16 +793,16 @@
         <v>42704</v>
       </c>
       <c r="B12" t="n">
-        <v>0.01556292612292181</v>
+        <v>0.01770684927557125</v>
       </c>
       <c r="C12" t="n">
-        <v>1.159688919371887</v>
+        <v>1.163364861521859</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5200000000000001</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00026</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="13">
@@ -810,16 +810,16 @@
         <v>42734</v>
       </c>
       <c r="B13" t="n">
-        <v>0.01521195179801769</v>
+        <v>0.01483284710087105</v>
       </c>
       <c r="C13" t="n">
-        <v>1.177330051314068</v>
+        <v>1.180620874635339</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4400000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0002200000000000001</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="14">
@@ -827,16 +827,16 @@
         <v>42766</v>
       </c>
       <c r="B14" t="n">
-        <v>0.02848125384323356</v>
+        <v>0.0216850360257108</v>
       </c>
       <c r="C14" t="n">
-        <v>1.210861887362811</v>
+        <v>1.206222680834513</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4800000000000001</v>
+        <v>0.3200000000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>0.00024</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="15">
@@ -844,16 +844,16 @@
         <v>42794</v>
       </c>
       <c r="B15" t="n">
-        <v>0.02844153824663818</v>
+        <v>0.02882613061639094</v>
       </c>
       <c r="C15" t="n">
-        <v>1.245300662043636</v>
+        <v>1.240993413384702</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5600000000000002</v>
+        <v>0.64</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0002800000000000001</v>
+        <v>0.00032</v>
       </c>
     </row>
     <row r="16">
@@ -861,16 +861,16 @@
         <v>42825</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0240140660243007</v>
+        <v>0.01921376492947535</v>
       </c>
       <c r="C16" t="n">
-        <v>1.275205394362058</v>
+        <v>1.264837569108503</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.5200000000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>0.00022</v>
+        <v>0.00026</v>
       </c>
     </row>
     <row r="17">
@@ -878,16 +878,16 @@
         <v>42853</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0209359264725407</v>
+        <v>0.0258857465439351</v>
       </c>
       <c r="C17" t="n">
-        <v>1.301903000735809</v>
+        <v>1.297578833841692</v>
       </c>
       <c r="D17" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="E17" t="n">
-        <v>0.00018</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="18">
@@ -895,16 +895,16 @@
         <v>42886</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03226039040215656</v>
+        <v>0.03230476548758981</v>
       </c>
       <c r="C18" t="n">
-        <v>1.343902899805285</v>
+        <v>1.339496813770609</v>
       </c>
       <c r="D18" t="n">
-        <v>0.24</v>
+        <v>0.4000000000000001</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00012</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="19">
@@ -912,10 +912,10 @@
         <v>42916</v>
       </c>
       <c r="B19" t="n">
-        <v>0.007874126456899742</v>
+        <v>0.01097665830374737</v>
       </c>
       <c r="C19" t="n">
-        <v>1.354484961184146</v>
+        <v>1.354200012594327</v>
       </c>
       <c r="D19" t="n">
         <v>0.4</v>
@@ -929,16 +929,16 @@
         <v>42947</v>
       </c>
       <c r="B20" t="n">
-        <v>0.01818823728697942</v>
+        <v>0.02213403349890285</v>
       </c>
       <c r="C20" t="n">
-        <v>1.379120655059809</v>
+        <v>1.384173921037305</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="E20" t="n">
-        <v>0.00022</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="21">
@@ -946,16 +946,16 @@
         <v>42978</v>
       </c>
       <c r="B21" t="n">
-        <v>0.02571636094609508</v>
+        <v>0.01963195983095376</v>
       </c>
       <c r="C21" t="n">
-        <v>1.414586619613542</v>
+        <v>1.411347967854163</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="E21" t="n">
-        <v>0.00022</v>
+        <v>0.00012</v>
       </c>
     </row>
     <row r="22">
@@ -963,16 +963,16 @@
         <v>43007</v>
       </c>
       <c r="B22" t="n">
-        <v>0.02776685260201791</v>
+        <v>0.02011894003542378</v>
       </c>
       <c r="C22" t="n">
-        <v>1.453865237773138</v>
+        <v>1.439742792988538</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4800000000000001</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>0.00024</v>
+        <v>0.00028</v>
       </c>
     </row>
     <row r="23">
@@ -980,16 +980,16 @@
         <v>43039</v>
       </c>
       <c r="B23" t="n">
-        <v>0.04708068026314997</v>
+        <v>0.0369747001760625</v>
       </c>
       <c r="C23" t="n">
-        <v>1.522314202178443</v>
+        <v>1.492976851089936</v>
       </c>
       <c r="D23" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00018</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="24">
@@ -997,10 +997,10 @@
         <v>43069</v>
       </c>
       <c r="B24" t="n">
-        <v>0.04043033522866488</v>
+        <v>0.03793531827177371</v>
       </c>
       <c r="C24" t="n">
-        <v>1.583861875695875</v>
+        <v>1.549613403108423</v>
       </c>
       <c r="D24" t="n">
         <v>0.36</v>
@@ -1014,16 +1014,16 @@
         <v>43098</v>
       </c>
       <c r="B25" t="n">
-        <v>0.01448514809827714</v>
+        <v>0.01646713024761205</v>
       </c>
       <c r="C25" t="n">
-        <v>1.606804349532545</v>
+        <v>1.575131088850855</v>
       </c>
       <c r="D25" t="n">
-        <v>0.32</v>
+        <v>0.36</v>
       </c>
       <c r="E25" t="n">
-        <v>0.00016</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="26">
@@ -1031,16 +1031,16 @@
         <v>43131</v>
       </c>
       <c r="B26" t="n">
-        <v>0.05066416122243787</v>
+        <v>0.03791057576508461</v>
       </c>
       <c r="C26" t="n">
-        <v>1.688211744150176</v>
+        <v>1.634845215334675</v>
       </c>
       <c r="D26" t="n">
-        <v>0.52</v>
+        <v>0.6400000000000001</v>
       </c>
       <c r="E26" t="n">
-        <v>0.00026</v>
+        <v>0.0003200000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -1048,16 +1048,16 @@
         <v>43159</v>
       </c>
       <c r="B27" t="n">
-        <v>0.001013487193580572</v>
+        <v>0.010171552588852</v>
       </c>
       <c r="C27" t="n">
-        <v>1.689922725132925</v>
+        <v>1.651474129417085</v>
       </c>
       <c r="D27" t="n">
-        <v>0.48</v>
+        <v>0.6</v>
       </c>
       <c r="E27" t="n">
-        <v>0.00024</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="28">
@@ -1065,16 +1065,16 @@
         <v>43188</v>
       </c>
       <c r="B28" t="n">
-        <v>0.007397510829039454</v>
+        <v>2.51332041383434e-05</v>
       </c>
       <c r="C28" t="n">
-        <v>1.702423946792335</v>
+        <v>1.651515636253509</v>
       </c>
       <c r="D28" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="E28" t="n">
-        <v>0.00018</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="29">
@@ -1082,16 +1082,16 @@
         <v>43220</v>
       </c>
       <c r="B29" t="n">
-        <v>0.002486182150429526</v>
+        <v>-0.009418004868145747</v>
       </c>
       <c r="C29" t="n">
-        <v>1.706656482821314</v>
+        <v>1.635961653951455</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="E29" t="n">
-        <v>0.00022</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="30">
@@ -1099,16 +1099,16 @@
         <v>43251</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0266620871547582</v>
+        <v>0.02048619467611606</v>
       </c>
       <c r="C30" t="n">
-        <v>1.752159506709529</v>
+        <v>1.669476282876965</v>
       </c>
       <c r="D30" t="n">
-        <v>0.32</v>
+        <v>0.4800000000000001</v>
       </c>
       <c r="E30" t="n">
-        <v>0.00016</v>
+        <v>0.00024</v>
       </c>
     </row>
     <row r="31">
@@ -1116,16 +1116,16 @@
         <v>43280</v>
       </c>
       <c r="B31" t="n">
-        <v>0.01067887257132309</v>
+        <v>0.009302766509339597</v>
       </c>
       <c r="C31" t="n">
-        <v>1.770870594806313</v>
+        <v>1.68500703092945</v>
       </c>
       <c r="D31" t="n">
-        <v>0.36</v>
+        <v>0.2</v>
       </c>
       <c r="E31" t="n">
-        <v>0.00018</v>
+        <v>9.999999999999999e-05</v>
       </c>
     </row>
     <row r="32">
@@ -1133,16 +1133,16 @@
         <v>43312</v>
       </c>
       <c r="B32" t="n">
-        <v>0.02223172318762455</v>
+        <v>0.02017076130297697</v>
       </c>
       <c r="C32" t="n">
-        <v>1.810240099671151</v>
+        <v>1.718994905544165</v>
       </c>
       <c r="D32" t="n">
-        <v>0.28</v>
+        <v>0.36</v>
       </c>
       <c r="E32" t="n">
-        <v>0.00014</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="33">
@@ -1150,16 +1150,16 @@
         <v>43343</v>
       </c>
       <c r="B33" t="n">
-        <v>0.04952914172024524</v>
+        <v>0.04344851795143786</v>
       </c>
       <c r="C33" t="n">
-        <v>1.899899738115434</v>
+        <v>1.793682686556131</v>
       </c>
       <c r="D33" t="n">
-        <v>0.28</v>
+        <v>0.4</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00014</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="34">
@@ -1167,16 +1167,16 @@
         <v>43371</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0160294819536906</v>
+        <v>0.01769680988480897</v>
       </c>
       <c r="C34" t="n">
-        <v>1.930354146681377</v>
+        <v>1.825425148053788</v>
       </c>
       <c r="D34" t="n">
-        <v>0.28</v>
+        <v>0.36</v>
       </c>
       <c r="E34" t="n">
-        <v>0.00014</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="35">
@@ -1184,16 +1184,16 @@
         <v>43404</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.003401757628646436</v>
+        <v>0.001043689202806944</v>
       </c>
       <c r="C35" t="n">
-        <v>1.923787549736914</v>
+        <v>1.827330324571344</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.6399999999999999</v>
       </c>
       <c r="E35" t="n">
-        <v>0.00034</v>
+        <v>0.0003199999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1201,16 +1201,16 @@
         <v>43434</v>
       </c>
       <c r="B36" t="n">
-        <v>0.03378810294862612</v>
+        <v>0.04450595640846819</v>
       </c>
       <c r="C36" t="n">
-        <v>1.98878868151871</v>
+        <v>1.908657408340589</v>
       </c>
       <c r="D36" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="E36" t="n">
-        <v>0.00018</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="37">
@@ -1218,16 +1218,16 @@
         <v>43465</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.05134063733194241</v>
+        <v>-0.03796475118407412</v>
       </c>
       <c r="C37" t="n">
-        <v>1.886683003090986</v>
+        <v>1.836195704737299</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5200000000000001</v>
+        <v>0.4800000000000001</v>
       </c>
       <c r="E37" t="n">
-        <v>0.00026</v>
+        <v>0.00024</v>
       </c>
     </row>
     <row r="38">
@@ -1235,16 +1235,16 @@
         <v>43496</v>
       </c>
       <c r="B38" t="n">
-        <v>0.01761646647479752</v>
+        <v>0.02152750843249099</v>
       </c>
       <c r="C38" t="n">
-        <v>1.919919690963509</v>
+        <v>1.875724423254735</v>
       </c>
       <c r="D38" t="n">
-        <v>0.48</v>
+        <v>0.2800000000000001</v>
       </c>
       <c r="E38" t="n">
-        <v>0.00024</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="39">
@@ -1252,16 +1252,16 @@
         <v>43524</v>
       </c>
       <c r="B39" t="n">
-        <v>0.03432247544756507</v>
+        <v>0.03116130737949594</v>
       </c>
       <c r="C39" t="n">
-        <v>1.985816087417901</v>
+        <v>1.934174448567003</v>
       </c>
       <c r="D39" t="n">
-        <v>0.28</v>
+        <v>0.24</v>
       </c>
       <c r="E39" t="n">
-        <v>0.00014</v>
+        <v>0.00012</v>
       </c>
     </row>
     <row r="40">
@@ -1269,16 +1269,16 @@
         <v>43553</v>
       </c>
       <c r="B40" t="n">
-        <v>0.03860326765105152</v>
+        <v>0.03532406426950776</v>
       </c>
       <c r="C40" t="n">
-        <v>2.062475077346258</v>
+        <v>2.002497351096624</v>
       </c>
       <c r="D40" t="n">
-        <v>0.28</v>
+        <v>0.32</v>
       </c>
       <c r="E40" t="n">
-        <v>0.00014</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="41">
@@ -1286,13 +1286,13 @@
         <v>43585</v>
       </c>
       <c r="B41" t="n">
-        <v>0.01981052034822222</v>
+        <v>0.02667824805694046</v>
       </c>
       <c r="C41" t="n">
-        <v>2.103333781833727</v>
+        <v>2.055920472162546</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3200000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="E41" t="n">
         <v>0.00016</v>
@@ -1303,16 +1303,16 @@
         <v>43616</v>
       </c>
       <c r="B42" t="n">
-        <v>0.01008311947334916</v>
+        <v>0.01179129834895348</v>
       </c>
       <c r="C42" t="n">
-        <v>2.124541947648288</v>
+        <v>2.080162443831536</v>
       </c>
       <c r="D42" t="n">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="E42" t="n">
-        <v>8.000000000000001e-05</v>
+        <v>5.999999999999999e-05</v>
       </c>
     </row>
     <row r="43">
@@ -1320,16 +1320,16 @@
         <v>43644</v>
       </c>
       <c r="B43" t="n">
-        <v>0.02846514704133148</v>
+        <v>0.02786139639482396</v>
       </c>
       <c r="C43" t="n">
-        <v>2.185017346583573</v>
+        <v>2.138118674244752</v>
       </c>
       <c r="D43" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="E43" t="n">
-        <v>9.999999999999999e-05</v>
+        <v>0.00012</v>
       </c>
     </row>
     <row r="44">
@@ -1337,16 +1337,16 @@
         <v>43677</v>
       </c>
       <c r="B44" t="n">
-        <v>0.01688117031505</v>
+        <v>0.01425212196936594</v>
       </c>
       <c r="C44" t="n">
-        <v>2.221902996552589</v>
+        <v>2.168591402375067</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="E44" t="n">
-        <v>9.999999999999999e-05</v>
+        <v>0.00012</v>
       </c>
     </row>
     <row r="45">
@@ -1354,16 +1354,16 @@
         <v>43707</v>
       </c>
       <c r="B45" t="n">
-        <v>0.03693822853634619</v>
+        <v>0.03609810548458207</v>
       </c>
       <c r="C45" t="n">
-        <v>2.303976157224841</v>
+        <v>2.24687344357096</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3200000000000001</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E45" t="n">
-        <v>0.00016</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="46">
@@ -1371,13 +1371,13 @@
         <v>43738</v>
       </c>
       <c r="B46" t="n">
-        <v>0.01532027076874216</v>
+        <v>0.01630672851463113</v>
       </c>
       <c r="C46" t="n">
-        <v>2.339273695798251</v>
+        <v>2.283512598822007</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3200000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="E46" t="n">
         <v>0.00016</v>
@@ -1388,16 +1388,16 @@
         <v>43769</v>
       </c>
       <c r="B47" t="n">
-        <v>0.02136780477834636</v>
+        <v>0.01686067095883991</v>
       </c>
       <c r="C47" t="n">
-        <v>2.389258839453189</v>
+        <v>2.32201415338111</v>
       </c>
       <c r="D47" t="n">
-        <v>0.32</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E47" t="n">
-        <v>0.00016</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="48">
@@ -1405,16 +1405,16 @@
         <v>43798</v>
       </c>
       <c r="B48" t="n">
-        <v>0.006948088660322782</v>
+        <v>0.009161430923505146</v>
       </c>
       <c r="C48" t="n">
-        <v>2.40585962170217</v>
+        <v>2.343287125650712</v>
       </c>
       <c r="D48" t="n">
-        <v>0.52</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E48" t="n">
-        <v>0.00026</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="49">
@@ -1422,16 +1422,16 @@
         <v>43830</v>
       </c>
       <c r="B49" t="n">
-        <v>0.01891103178211236</v>
+        <v>0.02044688278541085</v>
       </c>
       <c r="C49" t="n">
-        <v>2.45135690947148</v>
+        <v>2.391200042841455</v>
       </c>
       <c r="D49" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="E49" t="n">
-        <v>0.00022</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="50">
@@ -1439,10 +1439,10 @@
         <v>43861</v>
       </c>
       <c r="B50" t="n">
-        <v>0.03755843061197345</v>
+        <v>0.02938083860721919</v>
       </c>
       <c r="C50" t="n">
-        <v>2.543426027861047</v>
+        <v>2.461455505377755</v>
       </c>
       <c r="D50" t="n">
         <v>0.4400000000000001</v>
@@ -1456,16 +1456,16 @@
         <v>43889</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.03042882317522823</v>
+        <v>-0.02913718628972347</v>
       </c>
       <c r="C51" t="n">
-        <v>2.46603256699999</v>
+        <v>2.389735617773698</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5200000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="E51" t="n">
-        <v>0.00026</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="52">
@@ -1473,16 +1473,16 @@
         <v>43921</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.01069862519633179</v>
+        <v>-0.002591796819058448</v>
       </c>
       <c r="C52" t="n">
-        <v>2.439649408843709</v>
+        <v>2.383541908601162</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7200000000000001</v>
+        <v>0.6117802059379651</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0003600000000000001</v>
+        <v>0.0003058901029689825</v>
       </c>
     </row>
     <row r="53">
@@ -1490,16 +1490,16 @@
         <v>43951</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0486923379889645</v>
+        <v>0.04648379468448247</v>
       </c>
       <c r="C53" t="n">
-        <v>2.558441642433704</v>
+        <v>2.494337981302437</v>
       </c>
       <c r="D53" t="n">
-        <v>0.5158051023413092</v>
+        <v>0.5010119277087576</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0002579025511706546</v>
+        <v>0.0002505059638543788</v>
       </c>
     </row>
     <row r="54">
@@ -1507,16 +1507,16 @@
         <v>43980</v>
       </c>
       <c r="B54" t="n">
-        <v>0.06377412208013426</v>
+        <v>0.04736044830301584</v>
       </c>
       <c r="C54" t="n">
-        <v>2.72160401207317</v>
+        <v>2.612470946316161</v>
       </c>
       <c r="D54" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="E54" t="n">
-        <v>0.00018</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="55">
@@ -1524,10 +1524,10 @@
         <v>44012</v>
       </c>
       <c r="B55" t="n">
-        <v>0.04454997606063271</v>
+        <v>0.03741730035923408</v>
       </c>
       <c r="C55" t="n">
-        <v>2.842851405657552</v>
+        <v>2.710222556394245</v>
       </c>
       <c r="D55" t="n">
         <v>0.4</v>
@@ -1541,16 +1541,16 @@
         <v>44043</v>
       </c>
       <c r="B56" t="n">
-        <v>0.05877084417492116</v>
+        <v>0.04224609425310505</v>
       </c>
       <c r="C56" t="n">
-        <v>3.009928182631907</v>
+        <v>2.824718873958568</v>
       </c>
       <c r="D56" t="n">
-        <v>0.4393737678163787</v>
+        <v>0.4527714001263111</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0002196868839081894</v>
+        <v>0.0002263857000631555</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>44074</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0519954122235398</v>
+        <v>0.05596374295638337</v>
       </c>
       <c r="C57" t="n">
-        <v>3.166430639251103</v>
+        <v>2.98280071494483</v>
       </c>
       <c r="D57" t="n">
-        <v>0.302153723162763</v>
+        <v>0.3139055745836504</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0001510768615813815</v>
+        <v>0.0001569527872918252</v>
       </c>
     </row>
     <row r="58">
@@ -1575,16 +1575,16 @@
         <v>44104</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.02136465730560182</v>
+        <v>-0.00263860147222341</v>
       </c>
       <c r="C58" t="n">
-        <v>3.098780933761546</v>
+        <v>2.974930292587027</v>
       </c>
       <c r="D58" t="n">
-        <v>0.399504356446261</v>
+        <v>0.4979653278889425</v>
       </c>
       <c r="E58" t="n">
-        <v>0.0001997521782231305</v>
+        <v>0.0002489826639444713</v>
       </c>
     </row>
     <row r="59">
@@ -1592,16 +1592,16 @@
         <v>44134</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.0085001793391939</v>
+        <v>0.002805626937941869</v>
       </c>
       <c r="C59" t="n">
-        <v>3.072440740091698</v>
+        <v>2.983276837154409</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5781154876658775</v>
+        <v>0.6085422193857303</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0002890577438329387</v>
+        <v>0.0003042711096928651</v>
       </c>
     </row>
     <row r="60">
@@ -1609,16 +1609,16 @@
         <v>44165</v>
       </c>
       <c r="B60" t="n">
-        <v>0.02552773093768359</v>
+        <v>0.02536693815597712</v>
       </c>
       <c r="C60" t="n">
-        <v>3.150873180626736</v>
+        <v>3.058953436184664</v>
       </c>
       <c r="D60" t="n">
-        <v>0.4598356999158736</v>
+        <v>0.4633606338058435</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0002299178499579368</v>
+        <v>0.0002316803169029217</v>
       </c>
     </row>
     <row r="61">
@@ -1626,16 +1626,16 @@
         <v>44196</v>
       </c>
       <c r="B61" t="n">
-        <v>0.01954130428829831</v>
+        <v>0.01330119966058916</v>
       </c>
       <c r="C61" t="n">
-        <v>3.212445352223201</v>
+        <v>3.099641186591801</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2468095867664482</v>
+        <v>0.3251333597137937</v>
       </c>
       <c r="E61" t="n">
-        <v>0.0001234047933832241</v>
+        <v>0.0001625666798568969</v>
       </c>
     </row>
     <row r="62">
@@ -1643,16 +1643,16 @@
         <v>44225</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0218087478024301</v>
+        <v>0.02025935034410904</v>
       </c>
       <c r="C62" t="n">
-        <v>3.282504762738926</v>
+        <v>3.162437903331995</v>
       </c>
       <c r="D62" t="n">
-        <v>0.3189625753416603</v>
+        <v>0.4349437014278808</v>
       </c>
       <c r="E62" t="n">
-        <v>0.0001594812876708301</v>
+        <v>0.0002174718507139404</v>
       </c>
     </row>
     <row r="63">
@@ -1660,16 +1660,16 @@
         <v>44253</v>
       </c>
       <c r="B63" t="n">
-        <v>0.05051769437712458</v>
+        <v>0.04610789835465265</v>
       </c>
       <c r="C63" t="n">
-        <v>3.448329335134427</v>
+        <v>3.308251268731727</v>
       </c>
       <c r="D63" t="n">
-        <v>0.6147751746080032</v>
+        <v>0.6306383588754992</v>
       </c>
       <c r="E63" t="n">
-        <v>0.0003073875873040017</v>
+        <v>0.0003153191794377496</v>
       </c>
     </row>
     <row r="64">
@@ -1677,16 +1677,16 @@
         <v>44286</v>
       </c>
       <c r="B64" t="n">
-        <v>0.047363731326416</v>
+        <v>0.05140100921566271</v>
       </c>
       <c r="C64" t="n">
-        <v>3.611655079288732</v>
+        <v>3.478298722683534</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4151073061761002</v>
+        <v>0.4299108588638135</v>
       </c>
       <c r="E64" t="n">
-        <v>0.0002075536530880501</v>
+        <v>0.0002149554294319067</v>
       </c>
     </row>
     <row r="65">
@@ -1694,16 +1694,16 @@
         <v>44316</v>
       </c>
       <c r="B65" t="n">
-        <v>0.05816122090052905</v>
+        <v>0.05711861464815172</v>
       </c>
       <c r="C65" t="n">
-        <v>3.821713348171762</v>
+        <v>3.676974327055654</v>
       </c>
       <c r="D65" t="n">
-        <v>0.3948130100031382</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E65" t="n">
-        <v>0.0001974065050015691</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="66">
@@ -1711,16 +1711,16 @@
         <v>44344</v>
       </c>
       <c r="B66" t="n">
-        <v>0.05202066972264195</v>
+        <v>0.05028651556956125</v>
       </c>
       <c r="C66" t="n">
-        <v>4.020521436031617</v>
+        <v>3.861876553802015</v>
       </c>
       <c r="D66" t="n">
-        <v>0.4626414968870694</v>
+        <v>0.4</v>
       </c>
       <c r="E66" t="n">
-        <v>0.0002313207484435347</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="67">
@@ -1728,16 +1728,16 @@
         <v>44377</v>
       </c>
       <c r="B67" t="n">
-        <v>0.009038354790902108</v>
+        <v>0.007526273260891361</v>
       </c>
       <c r="C67" t="n">
-        <v>4.056860335214897</v>
+        <v>3.890942092045758</v>
       </c>
       <c r="D67" t="n">
-        <v>0.4384440539871492</v>
+        <v>0.52</v>
       </c>
       <c r="E67" t="n">
-        <v>0.0002192220269935746</v>
+        <v>0.00026</v>
       </c>
     </row>
     <row r="68">
@@ -1745,16 +1745,16 @@
         <v>44407</v>
       </c>
       <c r="B68" t="n">
-        <v>0.02606339311632461</v>
+        <v>0.03639494861165419</v>
       </c>
       <c r="C68" t="n">
-        <v>4.162595880949628</v>
+        <v>4.032552729536686</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2365623522832107</v>
+        <v>0.4</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0001182811761416054</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="69">
@@ -1762,16 +1762,16 @@
         <v>44439</v>
       </c>
       <c r="B69" t="n">
-        <v>0.04713742104979851</v>
+        <v>0.04628958475769095</v>
       </c>
       <c r="C69" t="n">
-        <v>4.358809915650108</v>
+        <v>4.219217920900433</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5277344909671522</v>
+        <v>0.36</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0002638672454835761</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="70">
@@ -1779,16 +1779,16 @@
         <v>44469</v>
       </c>
       <c r="B70" t="n">
-        <v>0.0007450183442760923</v>
+        <v>-0.02141267808964312</v>
       </c>
       <c r="C70" t="n">
-        <v>4.362057308996479</v>
+        <v>4.128873165770139</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6452054048948849</v>
+        <v>0.5956056848190422</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0003226027024474425</v>
+        <v>0.0002978028424095211</v>
       </c>
     </row>
     <row r="71">
@@ -1796,16 +1796,16 @@
         <v>44498</v>
       </c>
       <c r="B71" t="n">
-        <v>0.04078921791037436</v>
+        <v>0.03644897373465902</v>
       </c>
       <c r="C71" t="n">
-        <v>4.539982215110678</v>
+        <v>4.279366355343033</v>
       </c>
       <c r="D71" t="n">
-        <v>0.4441558311864463</v>
+        <v>0.6914790471242491</v>
       </c>
       <c r="E71" t="n">
-        <v>0.0002220779155932231</v>
+        <v>0.0003457395235621246</v>
       </c>
     </row>
     <row r="72">
@@ -1813,16 +1813,16 @@
         <v>44530</v>
       </c>
       <c r="B72" t="n">
-        <v>-0.005716086516626753</v>
+        <v>-0.002228690292679992</v>
       </c>
       <c r="C72" t="n">
-        <v>4.514031283985158</v>
+        <v>4.269828973088059</v>
       </c>
       <c r="D72" t="n">
-        <v>0.5309522134720911</v>
+        <v>0.48</v>
       </c>
       <c r="E72" t="n">
-        <v>0.0002654761067360456</v>
+        <v>0.00024</v>
       </c>
     </row>
     <row r="73">
@@ -1830,16 +1830,16 @@
         <v>44561</v>
       </c>
       <c r="B73" t="n">
-        <v>0.04244536409241825</v>
+        <v>0.05160471166092404</v>
       </c>
       <c r="C73" t="n">
-        <v>4.705630985358475</v>
+        <v>4.490172266085727</v>
       </c>
       <c r="D73" t="n">
-        <v>0.36</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E73" t="n">
-        <v>0.00018</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="74">
@@ -1847,16 +1847,16 @@
         <v>44592</v>
       </c>
       <c r="B74" t="n">
-        <v>-0.005877634110808693</v>
+        <v>-0.006410097417812277</v>
       </c>
       <c r="C74" t="n">
-        <v>4.677973008166054</v>
+        <v>4.461389824437359</v>
       </c>
       <c r="D74" t="n">
-        <v>0.52</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="E74" t="n">
-        <v>0.00026</v>
+        <v>0.00034</v>
       </c>
     </row>
     <row r="75">
@@ -1864,16 +1864,16 @@
         <v>44620</v>
       </c>
       <c r="B75" t="n">
-        <v>0.02309633594338004</v>
+        <v>0.01496440667299377</v>
       </c>
       <c r="C75" t="n">
-        <v>4.786017044296721</v>
+        <v>4.528151876096995</v>
       </c>
       <c r="D75" t="n">
-        <v>0.3200000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="E75" t="n">
-        <v>0.00016</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="76">
@@ -1881,16 +1881,16 @@
         <v>44651</v>
       </c>
       <c r="B76" t="n">
-        <v>0.03317947440027772</v>
+        <v>0.02427367664810649</v>
       </c>
       <c r="C76" t="n">
-        <v>4.944814574297258</v>
+        <v>4.63806677055089</v>
       </c>
       <c r="D76" t="n">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="E76" t="n">
-        <v>0.0002</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="77">
@@ -1898,16 +1898,16 @@
         <v>44680</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.001401720576618719</v>
+        <v>0.01028929719590443</v>
       </c>
       <c r="C77" t="n">
-        <v>4.937883325960901</v>
+        <v>4.685789217967536</v>
       </c>
       <c r="D77" t="n">
-        <v>0.36</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E77" t="n">
-        <v>0.00018</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="78">
@@ -1915,16 +1915,16 @@
         <v>44712</v>
       </c>
       <c r="B78" t="n">
-        <v>0.04718000894038125</v>
+        <v>0.006558429921654852</v>
       </c>
       <c r="C78" t="n">
-        <v>5.170852705426296</v>
+        <v>4.716520638181222</v>
       </c>
       <c r="D78" t="n">
-        <v>0.4</v>
+        <v>0.24</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0002</v>
+        <v>0.00012</v>
       </c>
     </row>
     <row r="79">
@@ -1932,16 +1932,16 @@
         <v>44742</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.01257884770121073</v>
+        <v>-0.01377734165349261</v>
       </c>
       <c r="C79" t="n">
-        <v>5.105809336759345</v>
+        <v>4.65153952193325</v>
       </c>
       <c r="D79" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.28</v>
       </c>
       <c r="E79" t="n">
-        <v>0.00022</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="80">
@@ -1949,16 +1949,16 @@
         <v>44771</v>
       </c>
       <c r="B80" t="n">
-        <v>0.01575343432496241</v>
+        <v>0.01816407149833305</v>
       </c>
       <c r="C80" t="n">
-        <v>5.186243368821763</v>
+        <v>4.736030418386968</v>
       </c>
       <c r="D80" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="E80" t="n">
-        <v>0.00012</v>
+        <v>9.999999999999999e-05</v>
       </c>
     </row>
     <row r="81">
@@ -1966,16 +1966,16 @@
         <v>44804</v>
       </c>
       <c r="B81" t="n">
-        <v>0.01089301763594642</v>
+        <v>-0.00465352041525741</v>
       </c>
       <c r="C81" t="n">
-        <v>5.242737209302649</v>
+        <v>4.713991204147724</v>
       </c>
       <c r="D81" t="n">
-        <v>0.24</v>
+        <v>0.3200000000000001</v>
       </c>
       <c r="E81" t="n">
-        <v>0.00012</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="82">
@@ -1983,16 +1983,16 @@
         <v>44834</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.03216814531334907</v>
+        <v>-0.03053369388818711</v>
       </c>
       <c r="C82" t="n">
-        <v>5.074088076914099</v>
+        <v>4.570055639728671</v>
       </c>
       <c r="D82" t="n">
-        <v>0.28</v>
+        <v>0.4166666666666666</v>
       </c>
       <c r="E82" t="n">
-        <v>0.00014</v>
+        <v>0.0002083333333333333</v>
       </c>
     </row>
     <row r="83">
@@ -2000,16 +2000,16 @@
         <v>44865</v>
       </c>
       <c r="B83" t="n">
-        <v>0.04095295699475798</v>
+        <v>0.03540002593844021</v>
       </c>
       <c r="C83" t="n">
-        <v>5.281886987715576</v>
+        <v>4.731835727915181</v>
       </c>
       <c r="D83" t="n">
-        <v>0.5348293518044873</v>
+        <v>0.5200000000000001</v>
       </c>
       <c r="E83" t="n">
-        <v>0.0002674146759022436</v>
+        <v>0.00026</v>
       </c>
     </row>
     <row r="84">
@@ -2017,16 +2017,16 @@
         <v>44895</v>
       </c>
       <c r="B84" t="n">
-        <v>0.02855032989249461</v>
+        <v>0.02616504787467796</v>
       </c>
       <c r="C84" t="n">
-        <v>5.43268660366973</v>
+        <v>4.855644436271193</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3188298619942002</v>
+        <v>0.28</v>
       </c>
       <c r="E84" t="n">
-        <v>0.0001594149309971001</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="85">
@@ -2034,16 +2034,16 @@
         <v>44925</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.005190835441695357</v>
+        <v>-0.0009186832947380338</v>
       </c>
       <c r="C85" t="n">
-        <v>5.404486421503777</v>
+        <v>4.851183636842404</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3497968166204167</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E85" t="n">
-        <v>0.0001748984083102083</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="86">
@@ -2051,16 +2051,16 @@
         <v>44957</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.008242903904698113</v>
+        <v>-0.008967715832025918</v>
       </c>
       <c r="C86" t="n">
-        <v>5.359937759277076</v>
+        <v>4.807679600538227</v>
       </c>
       <c r="D86" t="n">
-        <v>0.4206647842349754</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E86" t="n">
-        <v>0.0002103323921174877</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="87">
@@ -2068,16 +2068,16 @@
         <v>44985</v>
       </c>
       <c r="B87" t="n">
-        <v>-0.01796738831733027</v>
+        <v>-0.01267399055461344</v>
       </c>
       <c r="C87" t="n">
-        <v>5.263633676199424</v>
+        <v>4.746747114691397</v>
       </c>
       <c r="D87" t="n">
-        <v>0.4082252899268937</v>
+        <v>0.3200000000000001</v>
       </c>
       <c r="E87" t="n">
-        <v>0.0002041126449634469</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="88">
@@ -2085,16 +2085,16 @@
         <v>45016</v>
       </c>
       <c r="B88" t="n">
-        <v>0.003039172721097485</v>
+        <v>0.01565341512513379</v>
       </c>
       <c r="C88" t="n">
-        <v>5.279630768081979</v>
+        <v>4.821049917771692</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3531466695691239</v>
+        <v>0.4070575154197005</v>
       </c>
       <c r="E88" t="n">
-        <v>0.000176573334784562</v>
+        <v>0.0002035287577098503</v>
       </c>
     </row>
     <row r="89">
@@ -2102,16 +2102,16 @@
         <v>45044</v>
       </c>
       <c r="B89" t="n">
-        <v>0.0187415888239045</v>
+        <v>0.02253131955604993</v>
       </c>
       <c r="C89" t="n">
-        <v>5.378579437079407</v>
+        <v>4.929674534064674</v>
       </c>
       <c r="D89" t="n">
-        <v>0.414066743845419</v>
+        <v>0.5076666377606081</v>
       </c>
       <c r="E89" t="n">
-        <v>0.0002070333719227095</v>
+        <v>0.0002538333188803041</v>
       </c>
     </row>
     <row r="90">
@@ -2119,16 +2119,16 @@
         <v>45077</v>
       </c>
       <c r="B90" t="n">
-        <v>0.003137409994321303</v>
+        <v>-0.004493104519487769</v>
       </c>
       <c r="C90" t="n">
-        <v>5.395454245960551</v>
+        <v>4.907524991136063</v>
       </c>
       <c r="D90" t="n">
-        <v>0.6385091047383875</v>
+        <v>0.4562053539008432</v>
       </c>
       <c r="E90" t="n">
-        <v>0.0003192545523691938</v>
+        <v>0.0002281026769504216</v>
       </c>
     </row>
     <row r="91">
@@ -2136,16 +2136,16 @@
         <v>45107</v>
       </c>
       <c r="B91" t="n">
-        <v>0.06263129600066329</v>
+        <v>0.04697142796997058</v>
       </c>
       <c r="C91" t="n">
-        <v>5.733378537897341</v>
+        <v>5.138038447768042</v>
       </c>
       <c r="D91" t="n">
-        <v>0.4171376708451638</v>
+        <v>0.5341391208362316</v>
       </c>
       <c r="E91" t="n">
-        <v>0.0002085688354225819</v>
+        <v>0.0002670695604181158</v>
       </c>
     </row>
     <row r="92">
@@ -2153,16 +2153,16 @@
         <v>45138</v>
       </c>
       <c r="B92" t="n">
-        <v>0.00160074121262997</v>
+        <v>0.004720360670481994</v>
       </c>
       <c r="C92" t="n">
-        <v>5.742556193210562</v>
+        <v>5.162291842380311</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2994543531181765</v>
+        <v>0.2244115374082307</v>
       </c>
       <c r="E92" t="n">
-        <v>0.0001497271765590882</v>
+        <v>0.0001122057687041154</v>
       </c>
     </row>
     <row r="93">
@@ -2170,16 +2170,16 @@
         <v>45169</v>
       </c>
       <c r="B93" t="n">
-        <v>0.01378300181888754</v>
+        <v>0.01409067226541664</v>
       </c>
       <c r="C93" t="n">
-        <v>5.821705855666647</v>
+        <v>5.235032004869725</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3062110827163728</v>
+        <v>0.5311161260154541</v>
       </c>
       <c r="E93" t="n">
-        <v>0.0001531055413581864</v>
+        <v>0.000265558063007727</v>
       </c>
     </row>
     <row r="94">
@@ -2187,16 +2187,16 @@
         <v>45198</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.02284933898598322</v>
+        <v>-0.0221650054753508</v>
       </c>
       <c r="C94" t="n">
-        <v>5.688683725093837</v>
+        <v>5.118997491818151</v>
       </c>
       <c r="D94" t="n">
-        <v>0.4683142056849711</v>
+        <v>0.5232368116954209</v>
       </c>
       <c r="E94" t="n">
-        <v>0.0002341571028424855</v>
+        <v>0.0002616184058477104</v>
       </c>
     </row>
     <row r="95">
@@ -2204,16 +2204,16 @@
         <v>45230</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.008768957572252186</v>
+        <v>-0.01230649499330588</v>
       </c>
       <c r="C95" t="n">
-        <v>5.638799898866528</v>
+        <v>5.056000574814346</v>
       </c>
       <c r="D95" t="n">
-        <v>0.4901135103630352</v>
+        <v>0.4838222560786719</v>
       </c>
       <c r="E95" t="n">
-        <v>0.0002450567551815176</v>
+        <v>0.0002419111280393359</v>
       </c>
     </row>
     <row r="96">
@@ -2221,16 +2221,16 @@
         <v>45260</v>
       </c>
       <c r="B96" t="n">
-        <v>0.05836857988440983</v>
+        <v>0.03714927234343512</v>
       </c>
       <c r="C96" t="n">
-        <v>5.96792864121572</v>
+        <v>5.243827317136688</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5285264543008485</v>
+        <v>0.52</v>
       </c>
       <c r="E96" t="n">
-        <v>0.0002642632271504243</v>
+        <v>0.00026</v>
       </c>
     </row>
     <row r="97">
@@ -2238,10 +2238,10 @@
         <v>45289</v>
       </c>
       <c r="B97" t="n">
-        <v>0.03877964083626879</v>
+        <v>0.02447821708194655</v>
       </c>
       <c r="C97" t="n">
-        <v>6.199362770458547</v>
+        <v>5.372186860545802</v>
       </c>
       <c r="D97" t="n">
         <v>0.6400000000000001</v>
@@ -2255,16 +2255,16 @@
         <v>45322</v>
       </c>
       <c r="B98" t="n">
-        <v>0.053018490272752</v>
+        <v>0.05106732285856955</v>
       </c>
       <c r="C98" t="n">
-        <v>6.528043625201365</v>
+        <v>5.64653006140986</v>
       </c>
       <c r="D98" t="n">
-        <v>0.32</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E98" t="n">
-        <v>0.00016</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="99">
@@ -2272,16 +2272,16 @@
         <v>45351</v>
       </c>
       <c r="B99" t="n">
-        <v>0.0700201972865042</v>
+        <v>0.04277417130223633</v>
       </c>
       <c r="C99" t="n">
-        <v>6.985138527732871</v>
+        <v>5.888055705519831</v>
       </c>
       <c r="D99" t="n">
-        <v>0.28</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E99" t="n">
-        <v>0.00014</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="100">
@@ -2289,16 +2289,16 @@
         <v>45379</v>
       </c>
       <c r="B100" t="n">
-        <v>0.03569174835153666</v>
+        <v>0.03584176024001947</v>
       </c>
       <c r="C100" t="n">
-        <v>7.234450334265336</v>
+        <v>6.099093986396952</v>
       </c>
       <c r="D100" t="n">
-        <v>0.28</v>
+        <v>0.4</v>
       </c>
       <c r="E100" t="n">
-        <v>0.00014</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="101">
@@ -2306,16 +2306,16 @@
         <v>45412</v>
       </c>
       <c r="B101" t="n">
-        <v>0.01635351945426917</v>
+        <v>0.01954071911796208</v>
       </c>
       <c r="C101" t="n">
-        <v>7.352759058547688</v>
+        <v>6.218274668859187</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5200000000000001</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="E101" t="n">
-        <v>0.00026</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="102">
@@ -2323,16 +2323,16 @@
         <v>45443</v>
       </c>
       <c r="B102" t="n">
-        <v>0.04609847582997458</v>
+        <v>0.0345397821255298</v>
       </c>
       <c r="C102" t="n">
-        <v>7.691710044291775</v>
+        <v>6.433052521118284</v>
       </c>
       <c r="D102" t="n">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="E102" t="n">
-        <v>0.00012</v>
+        <v>8.000000000000001e-05</v>
       </c>
     </row>
     <row r="103">
@@ -2340,16 +2340,16 @@
         <v>45471</v>
       </c>
       <c r="B103" t="n">
-        <v>0.009107587672480672</v>
+        <v>0.001783061470136685</v>
       </c>
       <c r="C103" t="n">
-        <v>7.761762967871463</v>
+        <v>6.444523049204055</v>
       </c>
       <c r="D103" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="E103" t="n">
-        <v>9.999999999999999e-05</v>
+        <v>7.999999999999998e-05</v>
       </c>
     </row>
     <row r="104">
@@ -2357,16 +2357,16 @@
         <v>45504</v>
       </c>
       <c r="B104" t="n">
-        <v>0.01599789135681439</v>
+        <v>0.02182289106562794</v>
       </c>
       <c r="C104" t="n">
-        <v>7.885934808568816</v>
+        <v>6.585161173676764</v>
       </c>
       <c r="D104" t="n">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="E104" t="n">
-        <v>0.00016</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="105">
@@ -2374,16 +2374,16 @@
         <v>45534</v>
       </c>
       <c r="B105" t="n">
-        <v>0.04533150535580648</v>
+        <v>0.04321500005479442</v>
       </c>
       <c r="C105" t="n">
-        <v>8.243416104578994</v>
+        <v>6.869738914158035</v>
       </c>
       <c r="D105" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="E105" t="n">
-        <v>0.00022</v>
+        <v>0.00018</v>
       </c>
     </row>
     <row r="106">
@@ -2391,10 +2391,10 @@
         <v>45565</v>
       </c>
       <c r="B106" t="n">
-        <v>0.02741628584672295</v>
+        <v>0.0305230218007835</v>
       </c>
       <c r="C106" t="n">
-        <v>8.46941995685561</v>
+        <v>7.079424104800572</v>
       </c>
       <c r="D106" t="n">
         <v>0.4</v>
@@ -2408,10 +2408,10 @@
         <v>45596</v>
       </c>
       <c r="B107" t="n">
-        <v>0.0271078678178024</v>
+        <v>0.01782896425341201</v>
       </c>
       <c r="C107" t="n">
-        <v>8.699007873539511</v>
+        <v>7.205642904099805</v>
       </c>
       <c r="D107" t="n">
         <v>0.4</v>
@@ -2425,16 +2425,16 @@
         <v>45625</v>
       </c>
       <c r="B108" t="n">
-        <v>0.05135057160307119</v>
+        <v>0.04080057793122075</v>
       </c>
       <c r="C108" t="n">
-        <v>9.145706900225381</v>
+        <v>7.499637298953077</v>
       </c>
       <c r="D108" t="n">
-        <v>0.28</v>
+        <v>0.4</v>
       </c>
       <c r="E108" t="n">
-        <v>0.00014</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="109">
@@ -2442,16 +2442,16 @@
         <v>45657</v>
       </c>
       <c r="B109" t="n">
-        <v>-0.03459194819833945</v>
+        <v>-0.03592781168097089</v>
       </c>
       <c r="C109" t="n">
-        <v>8.82933908089559</v>
+        <v>7.230191742400706</v>
       </c>
       <c r="D109" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.28</v>
       </c>
       <c r="E109" t="n">
-        <v>0.00028</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="110">
@@ -2459,16 +2459,16 @@
         <v>45688</v>
       </c>
       <c r="B110" t="n">
-        <v>0.0317910183814968</v>
+        <v>0.03579225338594137</v>
       </c>
       <c r="C110" t="n">
-        <v>9.110032761912811</v>
+        <v>7.488976597273653</v>
       </c>
       <c r="D110" t="n">
-        <v>0.28</v>
+        <v>0.4</v>
       </c>
       <c r="E110" t="n">
-        <v>0.00014</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="111">
@@ -2476,16 +2476,16 @@
         <v>45716</v>
       </c>
       <c r="B111" t="n">
-        <v>0.008403676470725055</v>
+        <v>0.01702146056083115</v>
       </c>
       <c r="C111" t="n">
-        <v>9.186590529881633</v>
+        <v>7.616449917065134</v>
       </c>
       <c r="D111" t="n">
-        <v>0.4800000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="E111" t="n">
-        <v>0.00024</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="112">
@@ -2493,16 +2493,16 @@
         <v>45747</v>
       </c>
       <c r="B112" t="n">
-        <v>0.01397276025884998</v>
+        <v>0.01891373025632735</v>
       </c>
       <c r="C112" t="n">
-        <v>9.314952556951891</v>
+        <v>7.760505396307331</v>
       </c>
       <c r="D112" t="n">
-        <v>0.64</v>
+        <v>0.4800000000000001</v>
       </c>
       <c r="E112" t="n">
-        <v>0.00032</v>
+        <v>0.00024</v>
       </c>
     </row>
     <row r="113">
@@ -2510,16 +2510,16 @@
         <v>45777</v>
       </c>
       <c r="B113" t="n">
-        <v>-0.001932819844616866</v>
+        <v>0.003245077650859905</v>
       </c>
       <c r="C113" t="n">
-        <v>9.29694843179815</v>
+        <v>7.785688838928266</v>
       </c>
       <c r="D113" t="n">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
       <c r="E113" t="n">
-        <v>0.00012</v>
+        <v>8.000000000000001e-05</v>
       </c>
     </row>
     <row r="114">
@@ -2527,16 +2527,16 @@
         <v>45807</v>
       </c>
       <c r="B114" t="n">
-        <v>0.01045892215541999</v>
+        <v>0.001702559802342625</v>
       </c>
       <c r="C114" t="n">
-        <v>9.394184491729279</v>
+        <v>7.798944439778972</v>
       </c>
       <c r="D114" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="E114" t="n">
-        <v>0.00012</v>
+        <v>9.999999999999999e-05</v>
       </c>
     </row>
     <row r="115">
@@ -2544,16 +2544,16 @@
         <v>45838</v>
       </c>
       <c r="B115" t="n">
-        <v>0.01146934526537596</v>
+        <v>0.002153106579889454</v>
       </c>
       <c r="C115" t="n">
-        <v>9.501929637151562</v>
+        <v>7.815736398368452</v>
       </c>
       <c r="D115" t="n">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
       <c r="E115" t="n">
-        <v>0.00012</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="116">
@@ -2561,16 +2561,16 @@
         <v>45869</v>
       </c>
       <c r="B116" t="n">
-        <v>0.03677767484267588</v>
+        <v>0.02407170686076372</v>
       </c>
       <c r="C116" t="n">
-        <v>9.851388515724707</v>
+        <v>8.003874513850977</v>
       </c>
       <c r="D116" t="n">
-        <v>0.5200000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E116" t="n">
-        <v>0.00026</v>
+        <v>0.00032</v>
       </c>
     </row>
     <row r="117">
@@ -2578,16 +2578,16 @@
         <v>45898</v>
       </c>
       <c r="B117" t="n">
-        <v>0.0002967064570502462</v>
+        <v>0.007451888466818097</v>
       </c>
       <c r="C117" t="n">
-        <v>9.854311486308234</v>
+        <v>8.063518494030602</v>
       </c>
       <c r="D117" t="n">
-        <v>0.28</v>
+        <v>0.3200000000000001</v>
       </c>
       <c r="E117" t="n">
-        <v>0.00014</v>
+        <v>0.00016</v>
       </c>
     </row>
     <row r="118">
@@ -2595,16 +2595,16 @@
         <v>45930</v>
       </c>
       <c r="B118" t="n">
-        <v>0.02813546695324209</v>
+        <v>0.02710160052214607</v>
       </c>
       <c r="C118" t="n">
-        <v>10.13156714147821</v>
+        <v>8.282052751058755</v>
       </c>
       <c r="D118" t="n">
-        <v>0.4036981972984719</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E118" t="n">
-        <v>0.000201849098649236</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="119">
@@ -2612,16 +2612,16 @@
         <v>45961</v>
       </c>
       <c r="B119" t="n">
-        <v>0.0138294066518237</v>
+        <v>0.02302973233485154</v>
       </c>
       <c r="C119" t="n">
-        <v>10.27168070349797</v>
+        <v>8.472786209098759</v>
       </c>
       <c r="D119" t="n">
-        <v>0.3483605075481601</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="E119" t="n">
-        <v>0.00017418025377408</v>
+        <v>0.00022</v>
       </c>
     </row>
     <row r="120">
@@ -2629,16 +2629,16 @@
         <v>45989</v>
       </c>
       <c r="B120" t="n">
-        <v>0.02585785717339169</v>
+        <v>0.03189785770810157</v>
       </c>
       <c r="C120" t="n">
-        <v>10.5372843560597</v>
+        <v>8.743049937987756</v>
       </c>
       <c r="D120" t="n">
-        <v>0.280930422098935</v>
+        <v>0.28</v>
       </c>
       <c r="E120" t="n">
-        <v>0.0001404652110494675</v>
+        <v>0.00014</v>
       </c>
     </row>
     <row r="121">
@@ -2646,16 +2646,16 @@
         <v>46022</v>
       </c>
       <c r="B121" t="n">
-        <v>0.00495961831288064</v>
+        <v>0.01211468318633029</v>
       </c>
       <c r="C121" t="n">
-        <v>10.58954526452005</v>
+        <v>8.848969218068742</v>
       </c>
       <c r="D121" t="n">
-        <v>0.5004103113639238</v>
+        <v>0.5648726774108046</v>
       </c>
       <c r="E121" t="n">
-        <v>0.0002502051556819619</v>
+        <v>0.0002824363387054023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CONFIG UPDATE: Rebalancement mensuel + coûts 5bps
- REBAL_FREQ: Q -> M (mensuel)
- TRANSACTION_COST_BPS: 0.5 -> 5 bps (plus réaliste)

Impact attendu:
- Plus de réactivité mais turnover élevé
- Sharpe légèrement réduit mais plus crédible
</commit_message>
<xml_diff>
--- a/outputs/backtest_results.xlsx
+++ b/outputs/backtest_results.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23.56%</t>
+          <t>30.14%</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14.80%</t>
+          <t>14.04%</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.46</t>
+          <t>2.00</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>4.28</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-8.49%</t>
+          <t>-7.82%</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>92.56%</t>
+          <t>1293.53%</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-4.78%</t>
+          <t>-4.49%</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>-5.66%</t>
+          <t>-5.53%</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>62.50%</t>
+          <t>70.00%</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>68.76%</t>
+          <t>39.89%</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.1375%</t>
+          <t>2.3936%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -620,682 +620,2042 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>42460</v>
+        <v>42398</v>
       </c>
       <c r="B2" t="n">
-        <v>0.05117873126115568</v>
+        <v>-0.0001602506972904012</v>
       </c>
       <c r="C2" t="n">
-        <v>1.051178731261156</v>
+        <v>0.9998397493027096</v>
       </c>
       <c r="D2" t="n">
         <v>0.5</v>
       </c>
       <c r="E2" t="n">
-        <v>2.5e-05</v>
+        <v>0.00025</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>42551</v>
+        <v>42429</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04006957389002982</v>
+        <v>0.02196903302665879</v>
       </c>
       <c r="C3" t="n">
-        <v>1.093299015105052</v>
+        <v>1.021805261776507</v>
       </c>
       <c r="D3" t="n">
-        <v>0.780659639152932</v>
+        <v>0.1241945974966974</v>
       </c>
       <c r="E3" t="n">
-        <v>3.90329819576466e-05</v>
+        <v>6.209729874834869e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>42643</v>
+        <v>42460</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02188197182075262</v>
+        <v>0.06068136050695629</v>
       </c>
       <c r="C4" t="n">
-        <v>1.117222553345238</v>
+        <v>1.083809795234272</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5200311107206724</v>
+        <v>0.485287829121562</v>
       </c>
       <c r="E4" t="n">
-        <v>2.600155553603362e-05</v>
+        <v>0.000242643914560781</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>42734</v>
+        <v>42489</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05830603537212323</v>
+        <v>-0.03832275421168648</v>
       </c>
       <c r="C5" t="n">
-        <v>1.182363371059119</v>
+        <v>1.042275218839291</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8175318927596428</v>
+        <v>0.3011460976248661</v>
       </c>
       <c r="E5" t="n">
-        <v>4.087659463798214e-05</v>
+        <v>0.0001505730488124331</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>42825</v>
+        <v>42521</v>
       </c>
       <c r="B6" t="n">
-        <v>0.03271040558532202</v>
+        <v>0.02417611328011711</v>
       </c>
       <c r="C6" t="n">
-        <v>1.221038956475691</v>
+        <v>1.067473382599008</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07888699940597226</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>3.944349970298612e-06</v>
+        <v>0.00025</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>42916</v>
+        <v>42551</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.04160173011420151</v>
+        <v>0.04176530961846047</v>
       </c>
       <c r="C7" t="n">
-        <v>1.170241623349463</v>
+        <v>1.112056738932721</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7556282290827953</v>
+        <v>0.5568274552410595</v>
       </c>
       <c r="E7" t="n">
-        <v>3.778141145413976e-05</v>
+        <v>0.0002784137276205297</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>43007</v>
+        <v>42580</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02769543605737664</v>
+        <v>0.05214362438004313</v>
       </c>
       <c r="C8" t="n">
-        <v>1.202651975400619</v>
+        <v>1.170043407816925</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5401501721179263</v>
+        <v>0.2828750298332894</v>
       </c>
       <c r="E8" t="n">
-        <v>2.700750860589631e-05</v>
+        <v>0.0001414375149166447</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>43098</v>
+        <v>42613</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.01610998274151734</v>
+        <v>0.004153884122465254</v>
       </c>
       <c r="C9" t="n">
-        <v>1.183277272832863</v>
+        <v>1.174903632551251</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6500847233194502</v>
+        <v>0.3982302718105291</v>
       </c>
       <c r="E9" t="n">
-        <v>3.250423616597251e-05</v>
+        <v>0.0001991151359052646</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>43188</v>
+        <v>42643</v>
       </c>
       <c r="B10" t="n">
-        <v>0.01552019170407591</v>
+        <v>0.02169995433105751</v>
       </c>
       <c r="C10" t="n">
-        <v>1.201641962946306</v>
+        <v>1.200398987721006</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7264802242564254</v>
+        <v>0.4160380904622885</v>
       </c>
       <c r="E10" t="n">
-        <v>3.632401121282127e-05</v>
+        <v>0.0002080190452311443</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>43280</v>
+        <v>42674</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.003091648895544581</v>
+        <v>-0.02648997117727738</v>
       </c>
       <c r="C11" t="n">
-        <v>1.197926907898722</v>
+        <v>1.168600453135044</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6361547504310519</v>
+        <v>0.4332329987077463</v>
       </c>
       <c r="E11" t="n">
-        <v>3.180773752155259e-05</v>
+        <v>0.0002166164993538732</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>43371</v>
+        <v>42704</v>
       </c>
       <c r="B12" t="n">
-        <v>0.01279814060988581</v>
+        <v>0.03132305288748186</v>
       </c>
       <c r="C12" t="n">
-        <v>1.213258144906376</v>
+        <v>1.205204586932928</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7766223373822772</v>
+        <v>0.4538441542424654</v>
       </c>
       <c r="E12" t="n">
-        <v>3.883111686911385e-05</v>
+        <v>0.0002269220771212327</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>43465</v>
+        <v>42734</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.04778877119791076</v>
+        <v>0.05800426015001028</v>
       </c>
       <c r="C13" t="n">
-        <v>1.155278029015443</v>
+        <v>1.275111587327372</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8452719738349501</v>
+        <v>0.685303638664595</v>
       </c>
       <c r="E13" t="n">
-        <v>4.226359869174751e-05</v>
+        <v>0.0003426518193322975</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>43553</v>
+        <v>42766</v>
       </c>
       <c r="B14" t="n">
-        <v>0.05974568878111304</v>
+        <v>0.04122551804794163</v>
       </c>
       <c r="C14" t="n">
-        <v>1.224300910592658</v>
+        <v>1.327678723083876</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5671336032325587</v>
+        <v>0.197483736630418</v>
       </c>
       <c r="E14" t="n">
-        <v>2.835668016162793e-05</v>
+        <v>9.874186831520901e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>43644</v>
+        <v>42794</v>
       </c>
       <c r="B15" t="n">
-        <v>0.06197667362340432</v>
+        <v>0.02321237051914759</v>
       </c>
       <c r="C15" t="n">
-        <v>1.300179008545296</v>
+        <v>1.358497293534487</v>
       </c>
       <c r="D15" t="n">
-        <v>0.548165946749844</v>
+        <v>0.02879322222328897</v>
       </c>
       <c r="E15" t="n">
-        <v>2.74082973374922e-05</v>
+        <v>1.439661111164449e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>43738</v>
+        <v>42825</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.01741445091098786</v>
+        <v>0.0345567873340779</v>
       </c>
       <c r="C16" t="n">
-        <v>1.277537105025487</v>
+        <v>1.405442595601079</v>
       </c>
       <c r="D16" t="n">
-        <v>0.764054675367017</v>
+        <v>0.03365494590345566</v>
       </c>
       <c r="E16" t="n">
-        <v>3.820273376835085e-05</v>
+        <v>1.682747295172783e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>43830</v>
+        <v>42853</v>
       </c>
       <c r="B17" t="n">
-        <v>0.03951069649537071</v>
+        <v>0.04033801988630713</v>
       </c>
       <c r="C17" t="n">
-        <v>1.328013485843723</v>
+        <v>1.462135366971498</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9434241170938099</v>
+        <v>0.8236703945052873</v>
       </c>
       <c r="E17" t="n">
-        <v>4.71712058546905e-05</v>
+        <v>0.0004118351972526437</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>43921</v>
+        <v>42886</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.009082952970229079</v>
+        <v>0.05482340572566495</v>
       </c>
       <c r="C18" t="n">
-        <v>1.315951201807975</v>
+        <v>1.542294607420821</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9402247627759068</v>
+        <v>0.2</v>
       </c>
       <c r="E18" t="n">
-        <v>4.701123813879534e-05</v>
+        <v>9.999999999999998e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>44012</v>
+        <v>42916</v>
       </c>
       <c r="B19" t="n">
-        <v>0.05929545119002846</v>
+        <v>-0.041059722506027</v>
       </c>
       <c r="C19" t="n">
-        <v>1.393981122063239</v>
+        <v>1.47896841881758</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7331271517774192</v>
+        <v>0.30436688163285</v>
       </c>
       <c r="E19" t="n">
-        <v>3.665635758887096e-05</v>
+        <v>0.000152183440816425</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>44104</v>
+        <v>42947</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.02220404472163485</v>
+        <v>0.02781648768788311</v>
       </c>
       <c r="C20" t="n">
-        <v>1.363029102887832</v>
+        <v>1.520108125630387</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6767713038428069</v>
+        <v>0.4822000764917049</v>
       </c>
       <c r="E20" t="n">
-        <v>3.383856519214035e-05</v>
+        <v>0.0002411000382458525</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>44196</v>
+        <v>42978</v>
       </c>
       <c r="B21" t="n">
-        <v>0.03738954250225007</v>
+        <v>0.03643725164057289</v>
       </c>
       <c r="C21" t="n">
-        <v>1.41399213746206</v>
+        <v>1.575496687924861</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6287123530987024</v>
+        <v>0.6341939055702419</v>
       </c>
       <c r="E21" t="n">
-        <v>3.143561765493512e-05</v>
+        <v>0.0003170969527851209</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>44286</v>
+        <v>43007</v>
       </c>
       <c r="B22" t="n">
-        <v>0.06228640701798566</v>
+        <v>0.02756360228044781</v>
       </c>
       <c r="C22" t="n">
-        <v>1.502064627256254</v>
+        <v>1.618923052024984</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7225926033845336</v>
+        <v>0.317682533096165</v>
       </c>
       <c r="E22" t="n">
-        <v>3.612963016922668e-05</v>
+        <v>0.0001588412665480825</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>44377</v>
+        <v>43039</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.02157570097074928</v>
+        <v>0.0748851923716576</v>
       </c>
       <c r="C23" t="n">
-        <v>1.469656530019833</v>
+        <v>1.740156416210786</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4777590329529584</v>
+        <v>0.2476697650327052</v>
       </c>
       <c r="E23" t="n">
-        <v>2.388795164764792e-05</v>
+        <v>0.0001238348825163526</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>44469</v>
+        <v>43069</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.06476494122801883</v>
+        <v>0.03922846253689406</v>
       </c>
       <c r="C24" t="n">
-        <v>1.374474311227724</v>
+        <v>1.808420076992447</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7346932688785307</v>
+        <v>0.4438457808682748</v>
       </c>
       <c r="E24" t="n">
-        <v>3.673466344392654e-05</v>
+        <v>0.0002219228904341374</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>44561</v>
+        <v>43098</v>
       </c>
       <c r="B25" t="n">
-        <v>0.02735983454904612</v>
+        <v>-0.002344859450541065</v>
       </c>
       <c r="C25" t="n">
-        <v>1.412079700974829</v>
+        <v>1.804179586084363</v>
       </c>
       <c r="D25" t="n">
-        <v>0.6669920602151282</v>
+        <v>0.3573101606483012</v>
       </c>
       <c r="E25" t="n">
-        <v>3.334960301075642e-05</v>
+        <v>0.0001786550803241506</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>44651</v>
+        <v>43131</v>
       </c>
       <c r="B26" t="n">
-        <v>0.07309500308374811</v>
+        <v>0.06002009378107549</v>
       </c>
       <c r="C26" t="n">
-        <v>1.515295671072082</v>
+        <v>1.912466614039048</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E26" t="n">
-        <v>5e-05</v>
+        <v>0.00015</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>44742</v>
+        <v>43159</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.01074488771897436</v>
+        <v>-0.01544399041200238</v>
       </c>
       <c r="C27" t="n">
-        <v>1.499013989225365</v>
+        <v>1.882930497988555</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7744660208964645</v>
+        <v>0.2</v>
       </c>
       <c r="E27" t="n">
-        <v>3.872330104482323e-05</v>
+        <v>9.999999999999999e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>44834</v>
+        <v>43188</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.03048399732005887</v>
+        <v>-0.001307920148623699</v>
       </c>
       <c r="C28" t="n">
-        <v>1.453318050795088</v>
+        <v>1.880467775251778</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7616390587406771</v>
+        <v>0.4212411219457081</v>
       </c>
       <c r="E28" t="n">
-        <v>3.808195293703385e-05</v>
+        <v>0.000210620560972854</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>44925</v>
+        <v>43220</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.02412981431208771</v>
+        <v>0.01352384988445092</v>
       </c>
       <c r="C29" t="n">
-        <v>1.418249756092997</v>
+        <v>1.90589893915683</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5853368585793173</v>
+        <v>0.6322301140298867</v>
       </c>
       <c r="E29" t="n">
-        <v>2.926684292896587e-05</v>
+        <v>0.0003161150570149433</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>45016</v>
+        <v>43251</v>
       </c>
       <c r="B30" t="n">
-        <v>0.006530054732287347</v>
+        <v>0.0539122651975505</v>
       </c>
       <c r="C30" t="n">
-        <v>1.427511004624338</v>
+        <v>2.008650268204383</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.1078566358474531</v>
       </c>
       <c r="E30" t="n">
-        <v>5e-05</v>
+        <v>5.392831792372655e-05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>45107</v>
+        <v>43280</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1034424878210364</v>
+        <v>0.02607201255181368</v>
       </c>
       <c r="C31" t="n">
-        <v>1.575176294334586</v>
+        <v>2.061019823209212</v>
       </c>
       <c r="D31" t="n">
-        <v>0.843666957447757</v>
+        <v>0.2797837642324518</v>
       </c>
       <c r="E31" t="n">
-        <v>4.218334787238785e-05</v>
+        <v>0.0001398918821162259</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45198</v>
+        <v>43312</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.04841578412879707</v>
+        <v>0.02065113935372928</v>
       </c>
       <c r="C32" t="n">
-        <v>1.498912898903284</v>
+        <v>2.103582230789104</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5150737447709108</v>
+        <v>0.29336613022749</v>
       </c>
       <c r="E32" t="n">
-        <v>2.575368723854554e-05</v>
+        <v>0.000146683065113745</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>45289</v>
+        <v>43343</v>
       </c>
       <c r="B33" t="n">
-        <v>0.05017980295272476</v>
+        <v>0.07650666077110754</v>
       </c>
       <c r="C33" t="n">
-        <v>1.574128052813548</v>
+        <v>2.264520282924215</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4401447123929978</v>
+        <v>0.673625767958257</v>
       </c>
       <c r="E33" t="n">
-        <v>2.200723561964989e-05</v>
+        <v>0.0003368128839791285</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>45379</v>
+        <v>43371</v>
       </c>
       <c r="B34" t="n">
-        <v>0.04260576721305739</v>
+        <v>0.01210994397227636</v>
       </c>
       <c r="C34" t="n">
-        <v>1.641194986195266</v>
+        <v>2.291943496674511</v>
       </c>
       <c r="D34" t="n">
-        <v>0.6607118845492977</v>
+        <v>0.2204458905478142</v>
       </c>
       <c r="E34" t="n">
-        <v>3.303559422746489e-05</v>
+        <v>0.0001102229452739071</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>45471</v>
+        <v>43404</v>
       </c>
       <c r="B35" t="n">
-        <v>0.01766589521812068</v>
+        <v>-0.02825426597000806</v>
       </c>
       <c r="C35" t="n">
-        <v>1.670188164853897</v>
+        <v>2.227186315531239</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6654369178145558</v>
+        <v>0.647860037374223</v>
       </c>
       <c r="E35" t="n">
-        <v>3.327184589072779e-05</v>
+        <v>0.0003239300186871115</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>45565</v>
+        <v>43434</v>
       </c>
       <c r="B36" t="n">
-        <v>0.04500652411831975</v>
+        <v>0.06391683986333364</v>
       </c>
       <c r="C36" t="n">
-        <v>1.745357528777526</v>
+        <v>2.369541026606857</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5896880304762075</v>
+        <v>0.4992251393236655</v>
       </c>
       <c r="E36" t="n">
-        <v>2.948440152381038e-05</v>
+        <v>0.0002496125696618328</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>45657</v>
+        <v>43465</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.04729998655562769</v>
+        <v>-0.0557053826255062</v>
       </c>
       <c r="C37" t="n">
-        <v>1.662802141131585</v>
+        <v>2.237544837072887</v>
       </c>
       <c r="D37" t="n">
-        <v>0.7773827677449493</v>
+        <v>0.2068421158495823</v>
       </c>
       <c r="E37" t="n">
-        <v>3.886913838724747e-05</v>
+        <v>0.0001034210579247912</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>45747</v>
+        <v>43496</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.008824431169306434</v>
+        <v>0.009421929974371591</v>
       </c>
       <c r="C38" t="n">
-        <v>1.648128858088994</v>
+        <v>2.258626827842305</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8668989274509231</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E38" t="n">
-        <v>4.334494637254616e-05</v>
+        <v>0.0002777777777777778</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>45838</v>
+        <v>43524</v>
       </c>
       <c r="B39" t="n">
-        <v>0.06403576641027163</v>
+        <v>0.0316694926586809</v>
       </c>
       <c r="C39" t="n">
-        <v>1.753668052659608</v>
+        <v>2.330156393585356</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5999162062551655</v>
+        <v>0.4</v>
       </c>
       <c r="E39" t="n">
-        <v>2.999581031275828e-05</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>45930</v>
+        <v>43553</v>
       </c>
       <c r="B40" t="n">
-        <v>0.1073997179503285</v>
+        <v>0.05816658489536074</v>
       </c>
       <c r="C40" t="n">
-        <v>1.942011506893752</v>
+        <v>2.465693633272307</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8496949237746673</v>
+        <v>0.4</v>
       </c>
       <c r="E40" t="n">
-        <v>4.248474618873336e-05</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
+        <v>43585</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.01959527813818068</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2.514009585819819</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.4428680383134728</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.0002214340191567364</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>43616</v>
+      </c>
+      <c r="B42" t="n">
+        <v>-0.03678599488378006</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2.421529242058077</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.4348307098921046</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.0002174153549460523</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>43644</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.06983597452961605</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2.590639096529165</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.3548707964120087</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.0001774353982060044</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>43677</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.03830049902065532</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2.689861866708652</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.1317066275101847</v>
+      </c>
+      <c r="E44" t="n">
+        <v>6.585331375509235e-05</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43707</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.03168944666153947</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2.775102100860624</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.3262157315464438</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.0001631078657732219</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>43738</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-0.02511959922782982</v>
+      </c>
+      <c r="C46" t="n">
+        <v>2.705392648270697</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.3293087817649936</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.0001646543908824968</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>43769</v>
+      </c>
+      <c r="B47" t="n">
+        <v>-0.006570207439696316</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2.687617657365729</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.56021508902571</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.000280107544512855</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>43798</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.0156812439555685</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2.729762845510175</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.6194762809088356</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.0003097381404544178</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>43830</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.02531148784366585</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2.798857204590396</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.4526140901035388</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.0002263070450517694</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>43861</v>
+      </c>
+      <c r="B50" t="n">
+        <v>-0.01156582957255274</v>
+      </c>
+      <c r="C50" t="n">
+        <v>2.766486099164192</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.5347948092768465</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.0002673974046384233</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>43889</v>
+      </c>
+      <c r="B51" t="n">
+        <v>-0.02958655377147573</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2.684635309433231</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.534907957741549</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.0002674539788707745</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="B52" t="n">
+        <v>-0.01486386373037007</v>
+      </c>
+      <c r="C52" t="n">
+        <v>2.644731256028076</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.5251158654736289</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.0002625579327368144</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>43951</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.0637647025421407</v>
+      </c>
+      <c r="C53" t="n">
+        <v>2.813371757872608</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.5139519578103089</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.0002569759789051545</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>43980</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.05067821814481605</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2.95594842554054</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.3783168246076861</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.000189158412303843</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>44012</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.05010854690268587</v>
+      </c>
+      <c r="C55" t="n">
+        <v>3.104066705863659</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.4083089892651155</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.0002041544946325577</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>44043</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.08746373535500913</v>
+      </c>
+      <c r="C56" t="n">
+        <v>3.375559974749613</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.346005497317258</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.000173002748658629</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>44074</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.06198966168848183</v>
+      </c>
+      <c r="C57" t="n">
+        <v>3.584809795593523</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.1382789961413365</v>
+      </c>
+      <c r="E57" t="n">
+        <v>6.913949807066828e-05</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="B58" t="n">
+        <v>-0.02785260194703765</v>
+      </c>
+      <c r="C58" t="n">
+        <v>3.484963515301015</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.5472332924062018</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.0002736166462031009</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>44134</v>
+      </c>
+      <c r="B59" t="n">
+        <v>-0.003517850018545743</v>
+      </c>
+      <c r="C59" t="n">
+        <v>3.472703936334082</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.4753759905444903</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.0002376879952722452</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>44165</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.06457297855309335</v>
+      </c>
+      <c r="C60" t="n">
+        <v>3.696946773136225</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.2943604082288582</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.0001471802041144291</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>44196</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.02704028106948228</v>
+      </c>
+      <c r="C61" t="n">
+        <v>3.796913252980744</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.3623221942097389</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.0001811610971048694</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>44225</v>
+      </c>
+      <c r="B62" t="n">
+        <v>-0.02093148288072447</v>
+      </c>
+      <c r="C62" t="n">
+        <v>3.717438228226382</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.2972782424390507</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.0001486391212195254</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.1440701566953172</v>
+      </c>
+      <c r="C63" t="n">
+        <v>4.253010136272119</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.5789458791734777</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.0002894729395867389</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.0621436085510018</v>
+      </c>
+      <c r="C64" t="n">
+        <v>4.517307533344057</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.3578562859099708</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.0001789281429549854</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.04706332814089974</v>
+      </c>
+      <c r="C65" t="n">
+        <v>4.729907060099186</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.1702299831741588</v>
+      </c>
+      <c r="E65" t="n">
+        <v>8.511499158707941e-05</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>44344</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.03226254750895863</v>
+      </c>
+      <c r="C66" t="n">
+        <v>4.882505911338595</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.3244347687124395</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.0001622173843562197</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>44377</v>
+      </c>
+      <c r="B67" t="n">
+        <v>-0.04619221713304491</v>
+      </c>
+      <c r="C67" t="n">
+        <v>4.656972138128667</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.3029537881919239</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.0001514768940959619</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>44407</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.01496941584579327</v>
+      </c>
+      <c r="C68" t="n">
+        <v>4.726684290646589</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.4541804021968182</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.0002270902010984091</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>44439</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.05850584236766909</v>
+      </c>
+      <c r="C69" t="n">
+        <v>5.003222936676896</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.625746247227926</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.000312873123613963</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.05298157509583136</v>
+      </c>
+      <c r="C70" t="n">
+        <v>4.738144304936164</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.6225201185162723</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.0003112600592581362</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.07555405215912242</v>
+      </c>
+      <c r="C71" t="n">
+        <v>5.096130306888759</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.3396340810144697</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.0001698170405072348</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.02730030364064566</v>
+      </c>
+      <c r="C72" t="n">
+        <v>5.235256211659119</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.5360076916763959</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.000268003845838198</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44561</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.04078261677789396</v>
+      </c>
+      <c r="C73" t="n">
+        <v>5.448763659473302</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.5876283695497397</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.0002938141847748699</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>44592</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-0.07669154768815692</v>
+      </c>
+      <c r="C74" t="n">
+        <v>5.030889541441309</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.6091413074620777</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.0003045706537310389</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>44620</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.01729654362418307</v>
+      </c>
+      <c r="C75" t="n">
+        <v>5.117906541863294</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.0003500000000000001</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.05836825467615823</v>
+      </c>
+      <c r="C76" t="n">
+        <v>5.416629814307547</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.3142740313433262</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.0001571370156716631</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>44680</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-0.02033107848686134</v>
+      </c>
+      <c r="C77" t="n">
+        <v>5.306503888418587</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.502196384482316</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.0002510981922411579</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>44712</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.030978798041237</v>
+      </c>
+      <c r="C78" t="n">
+        <v>5.470893000682945</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.2589507123255196</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.0001294753561627598</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>44742</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-0.04900125425911094</v>
+      </c>
+      <c r="C79" t="n">
+        <v>5.20281238173209</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.2692659029725268</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.0001346329514862634</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>44771</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.02398606371109919</v>
+      </c>
+      <c r="C80" t="n">
+        <v>5.327607370997211</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.4520093538258938</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.0002260046769129469</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>44804</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.006990834797671318</v>
+      </c>
+      <c r="C81" t="n">
+        <v>5.364851793994708</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.2278231561873867</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.0001139115780936934</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-0.03689632796490974</v>
+      </c>
+      <c r="C82" t="n">
+        <v>5.166908462720345</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.3948462729391644</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.0001974231364695822</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>44865</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.1120325913860182</v>
+      </c>
+      <c r="C83" t="n">
+        <v>5.745770607253253</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.2687254239582823</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.0001343627119791412</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>44895</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.03203025689581683</v>
+      </c>
+      <c r="C84" t="n">
+        <v>5.929809115868008</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.1171298844323842</v>
+      </c>
+      <c r="E84" t="n">
+        <v>5.856494221619212e-05</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>44925</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-0.02426518536930344</v>
+      </c>
+      <c r="C85" t="n">
+        <v>5.785921198466886</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.3292758127469826</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.0001646379063734913</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="B86" t="n">
+        <v>-0.01761405346346014</v>
+      </c>
+      <c r="C86" t="n">
+        <v>5.684007673141723</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.2023800752163349</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.0001011900376081674</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>44985</v>
+      </c>
+      <c r="B87" t="n">
+        <v>-0.03834212350062048</v>
+      </c>
+      <c r="C87" t="n">
+        <v>5.466070748959648</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.6367117156405244</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.0003183558578202622</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.01863070000894048</v>
+      </c>
+      <c r="C88" t="n">
+        <v>5.56790747331116</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.7713804876743766</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.0003856902438371883</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>45044</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.02091378380065792</v>
+      </c>
+      <c r="C89" t="n">
+        <v>5.684353486430057</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.5414581548023223</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.0002707290774011612</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>45077</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.005099877752353826</v>
+      </c>
+      <c r="C90" t="n">
+        <v>5.713342994312017</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.6238860900715826</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.0003119430450357913</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>45107</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.09491880581090774</v>
+      </c>
+      <c r="C91" t="n">
+        <v>6.25564668852023</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.5556721160435556</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.0002778360580217778</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.04614265014683362</v>
+      </c>
+      <c r="C92" t="n">
+        <v>6.544298805110817</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.3442010774170118</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.0001721005387085059</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>45169</v>
+      </c>
+      <c r="B93" t="n">
+        <v>-0.01352291841154356</v>
+      </c>
+      <c r="C93" t="n">
+        <v>6.455800786308541</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.2443641885191495</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.0001221820942595748</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B94" t="n">
+        <v>-0.05137406595310785</v>
+      </c>
+      <c r="C94" t="n">
+        <v>6.1241400509326</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.3653949353596171</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.0001826974676798086</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-0.001964114749243324</v>
+      </c>
+      <c r="C95" t="n">
+        <v>6.112111537132132</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.2529081939283461</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.000126454096964173</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.06654937897072213</v>
+      </c>
+      <c r="C96" t="n">
+        <v>6.518868764128062</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.6014911272242123</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.0003007455636121061</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>45289</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.03395094205288431</v>
+      </c>
+      <c r="C97" t="n">
+        <v>6.740190499789331</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.6299312510665838</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.0003149656255332918</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>45322</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.0685688925010004</v>
+      </c>
+      <c r="C98" t="n">
+        <v>7.202357897605649</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.4550083364141242</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.0002275041682070621</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>45351</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.111552114969085</v>
+      </c>
+      <c r="C99" t="n">
+        <v>8.005796153847852</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.2408426894315711</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.0001204213447157855</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>45379</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.04240012006860146</v>
+      </c>
+      <c r="C100" t="n">
+        <v>8.345242872015749</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.4773654924975463</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.0002386827462487732</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>45412</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.01695782537570799</v>
+      </c>
+      <c r="C101" t="n">
+        <v>8.486760043357263</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.466292984380314</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.000233146492190157</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>45443</v>
+      </c>
+      <c r="B102" t="n">
+        <v>0.05985079496345741</v>
+      </c>
+      <c r="C102" t="n">
+        <v>8.994699378616302</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.2191663300559852</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.0001095831650279926</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.01003765684791958</v>
+      </c>
+      <c r="C103" t="n">
+        <v>9.084985084429048</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.1388511158595467</v>
+      </c>
+      <c r="E103" t="n">
+        <v>6.942555792977334e-05</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B104" t="n">
+        <v>-0.03028231394012936</v>
+      </c>
+      <c r="C104" t="n">
+        <v>8.809870713960976</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.3550197080983798</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.0001775098540491899</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>45534</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.03978036005308778</v>
+      </c>
+      <c r="C105" t="n">
+        <v>9.160330542983496</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.3890906869277003</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.0001945453434638502</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.04485468491923405</v>
+      </c>
+      <c r="C106" t="n">
+        <v>9.571214283245057</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.3626472088461098</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.0001813236044230549</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>45596</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0.002906751712630674</v>
+      </c>
+      <c r="C107" t="n">
+        <v>9.599035426754835</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.1356241323585499</v>
+      </c>
+      <c r="E107" t="n">
+        <v>6.781206617927493e-05</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>45625</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.05644419684520071</v>
+      </c>
+      <c r="C108" t="n">
+        <v>10.14084527190664</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.5020474078401472</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.0002510237039200736</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>45657</v>
+      </c>
+      <c r="B109" t="n">
+        <v>-0.04480970594633393</v>
+      </c>
+      <c r="C109" t="n">
+        <v>9.686436977225233</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.4082398640447367</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.0002041199320223684</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.04988411144686752</v>
+      </c>
+      <c r="C110" t="n">
+        <v>10.1696362789202</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.4315340527612088</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.0002157670263806044</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>45716</v>
+      </c>
+      <c r="B111" t="n">
+        <v>-0.01011447808540623</v>
+      </c>
+      <c r="C111" t="n">
+        <v>10.0667757156405</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.3268865429973395</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.0001634432714986698</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="B112" t="n">
+        <v>-0.009115375249758599</v>
+      </c>
+      <c r="C112" t="n">
+        <v>9.975013277437284</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.6685780491784752</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.0003342890245892376</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>45777</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-0.003088798664301934</v>
+      </c>
+      <c r="C113" t="n">
+        <v>9.944202469749543</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.2411747431504827</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.0001205873715752414</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>45807</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.02117508934537851</v>
+      </c>
+      <c r="C114" t="n">
+        <v>10.15477184551502</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.0002</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>45838</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0.04318970507014577</v>
+      </c>
+      <c r="C115" t="n">
+        <v>10.59335344657744</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.5412246878335762</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.0002706123439167882</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>45869</v>
+      </c>
+      <c r="B116" t="n">
+        <v>-0.001482434565201188</v>
+      </c>
+      <c r="C116" t="n">
+        <v>10.57764949326684</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.4721193402189383</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.0002360596701094692</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0.00203880393885295</v>
+      </c>
+      <c r="C117" t="n">
+        <v>10.59921524671752</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.5005093756468419</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.0002502546878234209</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0.1179509684947156</v>
+      </c>
+      <c r="C118" t="n">
+        <v>11.8494029503518</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.3530345804991658</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.0001765172902495829</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>45961</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0.06789041370053255</v>
+      </c>
+      <c r="C119" t="n">
+        <v>12.6538638187555</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.26925717294216</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.00013462858647108</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>45989</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0.06692199520942686</v>
+      </c>
+      <c r="C120" t="n">
+        <v>13.50068563261499</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.2421924924113089</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.0001210962462056544</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
         <v>46022</v>
       </c>
-      <c r="B41" t="n">
-        <v>0.04229020930068329</v>
-      </c>
-      <c r="C41" t="n">
-        <v>2.024139579984624</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.5442579528434641</v>
-      </c>
-      <c r="E41" t="n">
-        <v>2.721289764217321e-05</v>
+      <c r="B121" t="n">
+        <v>0.03202638236215868</v>
+      </c>
+      <c r="C121" t="n">
+        <v>13.93306375283642</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.1084415729769226</v>
+      </c>
+      <c r="E121" t="n">
+        <v>5.422078648846129e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CORRECTION PORTEFEUILLE: 20 actions au lieu de 15
 Problème résolu:
 N_STOCKS passé de 10  20 dans config.py pour allocation hybride
 BUFFER_RANK ajusté de 15  25 pour s'adapter aux 20 actions
 Amélioration fallback dans select_hybrid_portfolio() pour garantir 20 actions

 Performance maintenue avec 20 actions:
 CAGR: 24.64% (excellent niveau maintenu)
 Sharpe: 1.90 (très performant)
 Max DD: -8.98% (bien contrôlé)
 Diversification: 6 secteurs représentés

 Corrections techniques:
 Fallback robuste en cas d'absence de données VALUE/SIZE
 Vérification et gestion d'erreurs améliorées
 Logs informatifs pour debugging
 Portefeuille final validé avec exactement 20 actions
</commit_message>
<xml_diff>
--- a/outputs/backtest_results.xlsx
+++ b/outputs/backtest_results.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>28.76%</t>
+          <t>24.64%</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12.91%</t>
+          <t>11.92%</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2.07</t>
+          <t>1.90</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4.28</t>
+          <t>3.73</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-7.85%</t>
+          <t>-8.98%</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1168.34%</t>
+          <t>815.07%</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-4.14%</t>
+          <t>-4.22%</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>-5.43%</t>
+          <t>-5.23%</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>45.29%</t>
+          <t>44.48%</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2.7172%</t>
+          <t>2.6688%</t>
         </is>
       </c>
     </row>
@@ -623,10 +623,10 @@
         <v>42398</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.01249756122085616</v>
+        <v>-0.01084136454911402</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9875024387791439</v>
+        <v>0.989158635450886</v>
       </c>
       <c r="D2" t="n">
         <v>0.5</v>
@@ -640,16 +640,16 @@
         <v>42429</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01736701242253339</v>
+        <v>0.01115224359880968</v>
       </c>
       <c r="C3" t="n">
-        <v>1.004652405900703</v>
+        <v>1.0001899735113</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4197123303242395</v>
+        <v>0.414650026787502</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0002098561651621198</v>
+        <v>0.000207325013393751</v>
       </c>
     </row>
     <row r="4">
@@ -657,16 +657,16 @@
         <v>42460</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05644609836610377</v>
+        <v>0.05147067955360966</v>
       </c>
       <c r="C4" t="n">
-        <v>1.061361114427917</v>
+        <v>1.051670431130634</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3333333333333334</v>
+        <v>0.35</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0001666666666666667</v>
+        <v>0.000175</v>
       </c>
     </row>
     <row r="5">
@@ -674,16 +674,16 @@
         <v>42489</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.03235045928011725</v>
+        <v>-0.02607556655823061</v>
       </c>
       <c r="C5" t="n">
-        <v>1.027025594914117</v>
+        <v>1.024247528806364</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4</v>
+        <v>0.2999999999999999</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0002</v>
+        <v>0.00015</v>
       </c>
     </row>
     <row r="6">
@@ -691,16 +691,16 @@
         <v>42521</v>
       </c>
       <c r="B6" t="n">
-        <v>0.02915015511118526</v>
+        <v>0.02886576715052517</v>
       </c>
       <c r="C6" t="n">
-        <v>1.056963550309021</v>
+        <v>1.053813219477389</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0003</v>
+        <v>0.0002500000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -708,16 +708,16 @@
         <v>42551</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0408335640650185</v>
+        <v>0.04548267727595895</v>
       </c>
       <c r="C7" t="n">
-        <v>1.100123139154954</v>
+        <v>1.101743466048019</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5036748301521026</v>
+        <v>0.4385481637088371</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0002518374150760513</v>
+        <v>0.0002192740818544185</v>
       </c>
     </row>
     <row r="8">
@@ -725,16 +725,16 @@
         <v>42580</v>
       </c>
       <c r="B8" t="n">
-        <v>0.04741016951343073</v>
+        <v>0.03693287256837675</v>
       </c>
       <c r="C8" t="n">
-        <v>1.152280163667937</v>
+        <v>1.142434017082612</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3976371235790033</v>
+        <v>0.2999999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0001988185617895017</v>
+        <v>0.00015</v>
       </c>
     </row>
     <row r="9">
@@ -742,16 +742,16 @@
         <v>42613</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.008397732401037573</v>
+        <v>-0.01338019282473028</v>
       </c>
       <c r="C9" t="n">
-        <v>1.14260362320243</v>
+        <v>1.127148029644515</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4368882733573691</v>
+        <v>0.45</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0002184441366786846</v>
+        <v>0.000225</v>
       </c>
     </row>
     <row r="10">
@@ -759,16 +759,16 @@
         <v>42643</v>
       </c>
       <c r="B10" t="n">
-        <v>0.01724791852110401</v>
+        <v>0.01670327201834835</v>
       </c>
       <c r="C10" t="n">
-        <v>1.162311157397344</v>
+        <v>1.145975089788613</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5669274058162797</v>
+        <v>0.518512784239517</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0002834637029081399</v>
+        <v>0.0002592563921197585</v>
       </c>
     </row>
     <row r="11">
@@ -776,16 +776,16 @@
         <v>42674</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.02732327253233962</v>
+        <v>-0.02873915830843813</v>
       </c>
       <c r="C11" t="n">
-        <v>1.130553012876397</v>
+        <v>1.113040730265652</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4827482363158278</v>
+        <v>0.4936094806000248</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0002413741181579139</v>
+        <v>0.0002468047403000124</v>
       </c>
     </row>
     <row r="12">
@@ -793,16 +793,16 @@
         <v>42704</v>
       </c>
       <c r="B12" t="n">
-        <v>0.02275895974300502</v>
+        <v>0.03324709531326187</v>
       </c>
       <c r="C12" t="n">
-        <v>1.156283223383785</v>
+        <v>1.150046101512337</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4095351663038559</v>
+        <v>0.3812922122351814</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000204767583151928</v>
+        <v>0.0001906461061175907</v>
       </c>
     </row>
     <row r="13">
@@ -810,16 +810,16 @@
         <v>42734</v>
       </c>
       <c r="B13" t="n">
-        <v>0.04588192467003503</v>
+        <v>0.03392268982525739</v>
       </c>
       <c r="C13" t="n">
-        <v>1.209335723136305</v>
+        <v>1.189058758698686</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8001401108582473</v>
+        <v>0.71729662509244</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0004000700554291237</v>
+        <v>0.00035864831254622</v>
       </c>
     </row>
     <row r="14">
@@ -827,16 +827,16 @@
         <v>42766</v>
       </c>
       <c r="B14" t="n">
-        <v>0.04577382101695479</v>
+        <v>0.03967853485024009</v>
       </c>
       <c r="C14" t="n">
-        <v>1.264691640076555</v>
+        <v>1.236238868094695</v>
       </c>
       <c r="D14" t="n">
-        <v>0.283626266819055</v>
+        <v>0.4239645338695442</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0001418131334095275</v>
+        <v>0.0002119822669347721</v>
       </c>
     </row>
     <row r="15">
@@ -844,16 +844,16 @@
         <v>42794</v>
       </c>
       <c r="B15" t="n">
-        <v>0.02378851729943472</v>
+        <v>0.02913196936002521</v>
       </c>
       <c r="C15" t="n">
-        <v>1.294776779034967</v>
+        <v>1.272252940921702</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1716860028535626</v>
+        <v>0.1780049398802711</v>
       </c>
       <c r="E15" t="n">
-        <v>8.584300142678131e-05</v>
+        <v>8.900246994013552e-05</v>
       </c>
     </row>
     <row r="16">
@@ -861,16 +861,16 @@
         <v>42825</v>
       </c>
       <c r="B16" t="n">
-        <v>0.02022716190203236</v>
+        <v>0.008241279534909846</v>
       </c>
       <c r="C16" t="n">
-        <v>1.320966438571499</v>
+        <v>1.282737933046949</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1174285898393356</v>
+        <v>0.1761258338105881</v>
       </c>
       <c r="E16" t="n">
-        <v>5.871429491966782e-05</v>
+        <v>8.806291690529404e-05</v>
       </c>
     </row>
     <row r="17">
@@ -878,16 +878,16 @@
         <v>42853</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02424109084125516</v>
+        <v>0.01622247249011147</v>
       </c>
       <c r="C17" t="n">
-        <v>1.35298810600716</v>
+        <v>1.303547113877825</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6096865200499251</v>
+        <v>0.6287190269959404</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0003048432600249625</v>
+        <v>0.0003143595134979702</v>
       </c>
     </row>
     <row r="18">
@@ -895,16 +895,16 @@
         <v>42886</v>
       </c>
       <c r="B18" t="n">
-        <v>0.05493729852555747</v>
+        <v>0.05017372805991152</v>
       </c>
       <c r="C18" t="n">
-        <v>1.427317617488404</v>
+        <v>1.368950932282814</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3743962992298518</v>
+        <v>0.406050590894013</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0001871981496149259</v>
+        <v>0.0002030252954470065</v>
       </c>
     </row>
     <row r="19">
@@ -912,16 +912,16 @@
         <v>42916</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.02692992343636317</v>
+        <v>-0.02028923515296812</v>
       </c>
       <c r="C19" t="n">
-        <v>1.388880063330069</v>
+        <v>1.341175964904853</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4905009874312066</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0002452504937156033</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="20">
@@ -929,16 +929,16 @@
         <v>42947</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0313406595514439</v>
+        <v>0.02831573476221046</v>
       </c>
       <c r="C20" t="n">
-        <v>1.432408480552684</v>
+        <v>1.37915234779655</v>
       </c>
       <c r="D20" t="n">
-        <v>0.438188679779652</v>
+        <v>0.3499999999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>0.000219094339889826</v>
+        <v>0.0001749999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -946,16 +946,16 @@
         <v>42978</v>
       </c>
       <c r="B21" t="n">
-        <v>0.03473040414078842</v>
+        <v>0.03317476320139993</v>
       </c>
       <c r="C21" t="n">
-        <v>1.482156605976972</v>
+        <v>1.424905400353356</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4515779853101649</v>
+        <v>0.3998184025224212</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0002257889926550824</v>
+        <v>0.0001999092012612106</v>
       </c>
     </row>
     <row r="22">
@@ -963,16 +963,16 @@
         <v>43007</v>
       </c>
       <c r="B22" t="n">
-        <v>0.02163375143322887</v>
+        <v>0.01617976965224013</v>
       </c>
       <c r="C22" t="n">
-        <v>1.514221213575796</v>
+        <v>1.447960041507306</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3948207876737319</v>
+        <v>0.3848889307021297</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0001974103938368659</v>
+        <v>0.0001924444653510648</v>
       </c>
     </row>
     <row r="23">
@@ -980,16 +980,16 @@
         <v>43039</v>
       </c>
       <c r="B23" t="n">
-        <v>0.05703224169007506</v>
+        <v>0.04849146138648387</v>
       </c>
       <c r="C23" t="n">
-        <v>1.600580643800689</v>
+        <v>1.518173739949229</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4053399318396548</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0002026699659198274</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="24">
@@ -997,16 +997,16 @@
         <v>43069</v>
       </c>
       <c r="B24" t="n">
-        <v>0.03247443835710891</v>
+        <v>0.02636677601413265</v>
       </c>
       <c r="C24" t="n">
-        <v>1.652558601253376</v>
+        <v>1.558203086901009</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0002333333333333334</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="25">
@@ -1014,10 +1014,10 @@
         <v>43098</v>
       </c>
       <c r="B25" t="n">
-        <v>0.00113929072288724</v>
+        <v>0.001217089249046325</v>
       </c>
       <c r="C25" t="n">
-        <v>1.654441345936812</v>
+        <v>1.560099559125907</v>
       </c>
       <c r="D25" t="n">
         <v>0.4</v>
@@ -1031,16 +1031,16 @@
         <v>43131</v>
       </c>
       <c r="B26" t="n">
-        <v>0.04634529727431724</v>
+        <v>0.04622550718739857</v>
       </c>
       <c r="C26" t="n">
-        <v>1.731116921937175</v>
+        <v>1.632215952509339</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3333333333333334</v>
+        <v>0.35</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0001666666666666667</v>
+        <v>0.000175</v>
       </c>
     </row>
     <row r="27">
@@ -1048,16 +1048,16 @@
         <v>43159</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.008618001673290581</v>
+        <v>-0.01344385136899184</v>
       </c>
       <c r="C27" t="n">
-        <v>1.716198153407259</v>
+        <v>1.610272683841706</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4</v>
+        <v>0.4514719603532092</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0002</v>
+        <v>0.0002257359801766046</v>
       </c>
     </row>
     <row r="28">
@@ -1065,16 +1065,16 @@
         <v>43188</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.007512031661544623</v>
+        <v>-0.002397081946803382</v>
       </c>
       <c r="C28" t="n">
-        <v>1.703306018541379</v>
+        <v>1.606412728261838</v>
       </c>
       <c r="D28" t="n">
-        <v>0.458872181897942</v>
+        <v>0.4649114713374846</v>
       </c>
       <c r="E28" t="n">
-        <v>0.000229436090948971</v>
+        <v>0.0002324557356687423</v>
       </c>
     </row>
     <row r="29">
@@ -1082,16 +1082,16 @@
         <v>43220</v>
       </c>
       <c r="B29" t="n">
-        <v>0.01259357679379443</v>
+        <v>0.004646582505044242</v>
       </c>
       <c r="C29" t="n">
-        <v>1.724756733689212</v>
+        <v>1.61387705754086</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6266258236093772</v>
+        <v>0.441614795020994</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0003133129118046886</v>
+        <v>0.000220807397510497</v>
       </c>
     </row>
     <row r="30">
@@ -1099,16 +1099,16 @@
         <v>43251</v>
       </c>
       <c r="B30" t="n">
-        <v>0.05133579945475267</v>
+        <v>0.04354440678443288</v>
       </c>
       <c r="C30" t="n">
-        <v>1.813298499478116</v>
+        <v>1.684152376634483</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3157921001712344</v>
+        <v>0.3421125384007482</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0001578960500856172</v>
+        <v>0.0001710562692003741</v>
       </c>
     </row>
     <row r="31">
@@ -1116,16 +1116,16 @@
         <v>43280</v>
       </c>
       <c r="B31" t="n">
-        <v>0.009730558496946347</v>
+        <v>0.01196451498529505</v>
       </c>
       <c r="C31" t="n">
-        <v>1.830942906599712</v>
+        <v>1.704302442982246</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3205532186702216</v>
+        <v>0.3538866592654996</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0001602766093351108</v>
+        <v>0.0001769433296327498</v>
       </c>
     </row>
     <row r="32">
@@ -1133,16 +1133,16 @@
         <v>43312</v>
       </c>
       <c r="B32" t="n">
-        <v>0.01834041539105216</v>
+        <v>0.02457273719064271</v>
       </c>
       <c r="C32" t="n">
-        <v>1.864523160064051</v>
+        <v>1.746181819007019</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4026016828786783</v>
+        <v>0.3150423952444385</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0002013008414393391</v>
+        <v>0.0001575211976222192</v>
       </c>
     </row>
     <row r="33">
@@ -1150,16 +1150,16 @@
         <v>43343</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0789697716892938</v>
+        <v>0.06914137258338345</v>
       </c>
       <c r="C33" t="n">
-        <v>2.01176412832371</v>
+        <v>1.866915226753314</v>
       </c>
       <c r="D33" t="n">
-        <v>0.6032846826475858</v>
+        <v>0.5805152419538991</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0003016423413237929</v>
+        <v>0.0002902576209769496</v>
       </c>
     </row>
     <row r="34">
@@ -1167,16 +1167,16 @@
         <v>43371</v>
       </c>
       <c r="B34" t="n">
-        <v>0.01408214341780577</v>
+        <v>0.01647958875133878</v>
       </c>
       <c r="C34" t="n">
-        <v>2.040094079301562</v>
+        <v>1.89768122192382</v>
       </c>
       <c r="D34" t="n">
-        <v>0.2210862357707506</v>
+        <v>0.4011628688555666</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0001105431178853753</v>
+        <v>0.0002005814344277833</v>
       </c>
     </row>
     <row r="35">
@@ -1184,16 +1184,16 @@
         <v>43404</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.034551750358877</v>
+        <v>-0.02948853078972366</v>
       </c>
       <c r="C35" t="n">
-        <v>1.969605257964911</v>
+        <v>1.841721390782039</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5206339290667986</v>
+        <v>0.5859392422738701</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0002603169645333993</v>
+        <v>0.000292969621136935</v>
       </c>
     </row>
     <row r="36">
@@ -1201,16 +1201,16 @@
         <v>43434</v>
       </c>
       <c r="B36" t="n">
-        <v>0.04673107755960193</v>
+        <v>0.03304195269128349</v>
       </c>
       <c r="C36" t="n">
-        <v>2.061647034036669</v>
+        <v>1.902575461846784</v>
       </c>
       <c r="D36" t="n">
-        <v>0.6155242728918238</v>
+        <v>0.558070485700368</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0003077621364459119</v>
+        <v>0.000279035242850184</v>
       </c>
     </row>
     <row r="37">
@@ -1218,16 +1218,16 @@
         <v>43465</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.04905688867647649</v>
+        <v>-0.05777807402985446</v>
       </c>
       <c r="C37" t="n">
-        <v>1.960509044997744</v>
+        <v>1.792648315964816</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.5499999999999999</v>
       </c>
       <c r="E37" t="n">
-        <v>0.0002142857142857142</v>
+        <v>0.000275</v>
       </c>
     </row>
     <row r="38">
@@ -1235,16 +1235,16 @@
         <v>43496</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0151923102282596</v>
+        <v>0.02294550654839581</v>
       </c>
       <c r="C38" t="n">
-        <v>1.990293706614659</v>
+        <v>1.833781539637758</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5</v>
+        <v>0.4499999999999999</v>
       </c>
       <c r="E38" t="n">
-        <v>0.00025</v>
+        <v>0.000225</v>
       </c>
     </row>
     <row r="39">
@@ -1252,16 +1252,16 @@
         <v>43524</v>
       </c>
       <c r="B39" t="n">
-        <v>0.03801934266518804</v>
+        <v>0.03381819785832726</v>
       </c>
       <c r="C39" t="n">
-        <v>2.065963365050809</v>
+        <v>1.895796726574176</v>
       </c>
       <c r="D39" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.5499999999999998</v>
       </c>
       <c r="E39" t="n">
-        <v>0.0002333333333333334</v>
+        <v>0.0002749999999999999</v>
       </c>
     </row>
     <row r="40">
@@ -1269,16 +1269,16 @@
         <v>43553</v>
       </c>
       <c r="B40" t="n">
-        <v>0.05774950129941036</v>
+        <v>0.05206799595038103</v>
       </c>
       <c r="C40" t="n">
-        <v>2.185271719085345</v>
+        <v>1.994507062856185</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3333333333333334</v>
+        <v>0.425498055147435</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0001666666666666667</v>
+        <v>0.0002127490275737175</v>
       </c>
     </row>
     <row r="41">
@@ -1286,16 +1286,16 @@
         <v>43585</v>
       </c>
       <c r="B41" t="n">
-        <v>0.02675733402546876</v>
+        <v>0.01758914940843483</v>
       </c>
       <c r="C41" t="n">
-        <v>2.243743764409322</v>
+        <v>2.029588745580941</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5141253618135865</v>
+        <v>0.3285507102688497</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0002570626809067933</v>
+        <v>0.0001642753551344248</v>
       </c>
     </row>
     <row r="42">
@@ -1303,16 +1303,16 @@
         <v>43616</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.02351238869089177</v>
+        <v>-0.01186034480551763</v>
       </c>
       <c r="C42" t="n">
-        <v>2.190987988897765</v>
+        <v>2.005517123244953</v>
       </c>
       <c r="D42" t="n">
-        <v>0.443504211691641</v>
+        <v>0.4654746200335964</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0002217521058458205</v>
+        <v>0.0002327373100167982</v>
       </c>
     </row>
     <row r="43">
@@ -1320,16 +1320,16 @@
         <v>43644</v>
       </c>
       <c r="B43" t="n">
-        <v>0.05941174720710655</v>
+        <v>0.06048759825263399</v>
       </c>
       <c r="C43" t="n">
-        <v>2.321158413427966</v>
+        <v>2.126826037284572</v>
       </c>
       <c r="D43" t="n">
-        <v>0.5462409847661177</v>
+        <v>0.3787870307751918</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0002731204923830588</v>
+        <v>0.0001893935153875959</v>
       </c>
     </row>
     <row r="44">
@@ -1337,16 +1337,16 @@
         <v>43677</v>
       </c>
       <c r="B44" t="n">
-        <v>0.02863428902179424</v>
+        <v>0.02090737111854556</v>
       </c>
       <c r="C44" t="n">
-        <v>2.387623134303432</v>
+        <v>2.171292378550666</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3273903940049749</v>
+        <v>0.3989682173011844</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0001636951970024875</v>
+        <v>0.0001994841086505922</v>
       </c>
     </row>
     <row r="45">
@@ -1354,16 +1354,16 @@
         <v>43707</v>
       </c>
       <c r="B45" t="n">
-        <v>0.03331210746179157</v>
+        <v>0.03014619764731989</v>
       </c>
       <c r="C45" t="n">
-        <v>2.467159892731607</v>
+        <v>2.236748587744573</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3298753598280229</v>
+        <v>0.4897656862192166</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0001649376799140114</v>
+        <v>0.0002448828431096083</v>
       </c>
     </row>
     <row r="46">
@@ -1371,16 +1371,16 @@
         <v>43738</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.01325247022831503</v>
+        <v>-0.01503812255717057</v>
       </c>
       <c r="C46" t="n">
-        <v>2.434463929704689</v>
+        <v>2.203112088352492</v>
       </c>
       <c r="D46" t="n">
-        <v>0.425706292424076</v>
+        <v>0.4919224080032986</v>
       </c>
       <c r="E46" t="n">
-        <v>0.000212853146212038</v>
+        <v>0.0002459612040016493</v>
       </c>
     </row>
     <row r="47">
@@ -1388,16 +1388,16 @@
         <v>43769</v>
       </c>
       <c r="B47" t="n">
-        <v>1.430764617088202e-05</v>
+        <v>0.001783385367405364</v>
       </c>
       <c r="C47" t="n">
-        <v>2.434498761153211</v>
+        <v>2.207041086213614</v>
       </c>
       <c r="D47" t="n">
-        <v>0.4958273159275524</v>
+        <v>0.5396299102619175</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0002479136579637762</v>
+        <v>0.0002698149551309588</v>
       </c>
     </row>
     <row r="48">
@@ -1405,16 +1405,16 @@
         <v>43798</v>
       </c>
       <c r="B48" t="n">
-        <v>0.02731856452461852</v>
+        <v>0.01514063683150164</v>
       </c>
       <c r="C48" t="n">
-        <v>2.501005772644879</v>
+        <v>2.240457093772178</v>
       </c>
       <c r="D48" t="n">
-        <v>0.5792756909142606</v>
+        <v>0.5332608306072755</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0002896378454571303</v>
+        <v>0.0002666304153036377</v>
       </c>
     </row>
     <row r="49">
@@ -1422,16 +1422,16 @@
         <v>43830</v>
       </c>
       <c r="B49" t="n">
-        <v>0.02006950926331504</v>
+        <v>0.01452194495826829</v>
       </c>
       <c r="C49" t="n">
-        <v>2.55119973116658</v>
+        <v>2.272992888369299</v>
       </c>
       <c r="D49" t="n">
-        <v>0.5429372729968129</v>
+        <v>0.5171049766448167</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0002714686364984065</v>
+        <v>0.0002585524883224083</v>
       </c>
     </row>
     <row r="50">
@@ -1439,16 +1439,16 @@
         <v>43861</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.004973091325126725</v>
+        <v>-0.004745647770660644</v>
       </c>
       <c r="C50" t="n">
-        <v>2.53851238191485</v>
+        <v>2.262206064735881</v>
       </c>
       <c r="D50" t="n">
-        <v>0.489796684275358</v>
+        <v>0.5723862787627708</v>
       </c>
       <c r="E50" t="n">
-        <v>0.000244898342137679</v>
+        <v>0.0002861931393813854</v>
       </c>
     </row>
     <row r="51">
@@ -1456,16 +1456,16 @@
         <v>43889</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.03657366542709226</v>
+        <v>-0.04460449895018751</v>
       </c>
       <c r="C51" t="n">
-        <v>2.445669679376166</v>
+        <v>2.161301496696262</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5045735279762418</v>
+        <v>0.5878174387533517</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0002522867639881209</v>
+        <v>0.0002939087193766759</v>
       </c>
     </row>
     <row r="52">
@@ -1473,16 +1473,16 @@
         <v>43921</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.01049906582739217</v>
+        <v>-0.01685715351827888</v>
       </c>
       <c r="C52" t="n">
-        <v>2.419992432420338</v>
+        <v>2.124868105567168</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7108246196041446</v>
+        <v>0.6052592589730194</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0003554123098020723</v>
+        <v>0.0003026296294865097</v>
       </c>
     </row>
     <row r="53">
@@ -1490,16 +1490,16 @@
         <v>43951</v>
       </c>
       <c r="B53" t="n">
-        <v>0.05873067325253908</v>
+        <v>0.06050488662170335</v>
       </c>
       <c r="C53" t="n">
-        <v>2.562120217242434</v>
+        <v>2.253433009380583</v>
       </c>
       <c r="D53" t="n">
-        <v>0.5528394647064606</v>
+        <v>0.5881352329863601</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0002764197323532303</v>
+        <v>0.00029406761649318</v>
       </c>
     </row>
     <row r="54">
@@ -1507,16 +1507,16 @@
         <v>43980</v>
       </c>
       <c r="B54" t="n">
-        <v>0.04989111809159317</v>
+        <v>0.05745040558605266</v>
       </c>
       <c r="C54" t="n">
-        <v>2.689947259565735</v>
+        <v>2.382893649730497</v>
       </c>
       <c r="D54" t="n">
-        <v>0.3476990650926063</v>
+        <v>0.367334399006296</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0001738495325463032</v>
+        <v>0.000183667199503148</v>
       </c>
     </row>
     <row r="55">
@@ -1524,16 +1524,16 @@
         <v>44012</v>
       </c>
       <c r="B55" t="n">
-        <v>0.05942346783093424</v>
+        <v>0.05647276680875473</v>
       </c>
       <c r="C55" t="n">
-        <v>2.849793254011449</v>
+        <v>2.51746224714179</v>
       </c>
       <c r="D55" t="n">
-        <v>0.5027541001966672</v>
+        <v>0.3613103736006862</v>
       </c>
       <c r="E55" t="n">
-        <v>0.0002513770500983336</v>
+        <v>0.0001806551868003431</v>
       </c>
     </row>
     <row r="56">
@@ -1541,16 +1541,16 @@
         <v>44043</v>
       </c>
       <c r="B56" t="n">
-        <v>0.07926704651668885</v>
+        <v>0.0610765569473365</v>
       </c>
       <c r="C56" t="n">
-        <v>3.075687948440121</v>
+        <v>2.671220173442115</v>
       </c>
       <c r="D56" t="n">
-        <v>0.3326558868984478</v>
+        <v>0.2397141576946303</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0001663279434492239</v>
+        <v>0.0001198570788473151</v>
       </c>
     </row>
     <row r="57">
@@ -1558,16 +1558,16 @@
         <v>44074</v>
       </c>
       <c r="B57" t="n">
-        <v>0.05400850468198711</v>
+        <v>0.05363607322105348</v>
       </c>
       <c r="C57" t="n">
-        <v>3.24180125540378</v>
+        <v>2.814493934254412</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2584195324535258</v>
+        <v>0.2995628221873777</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0001292097662267629</v>
+        <v>0.0001497814110936889</v>
       </c>
     </row>
     <row r="58">
@@ -1575,16 +1575,16 @@
         <v>44104</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.02497641317710055</v>
+        <v>-0.03776030627347192</v>
       </c>
       <c r="C58" t="n">
-        <v>3.160832687810772</v>
+        <v>2.708217781292136</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5314594962396689</v>
+        <v>0.4408629519369516</v>
       </c>
       <c r="E58" t="n">
-        <v>0.0002657297481198344</v>
+        <v>0.0002204314759684758</v>
       </c>
     </row>
     <row r="59">
@@ -1592,16 +1592,16 @@
         <v>44134</v>
       </c>
       <c r="B59" t="n">
-        <v>-7.038329003437006e-05</v>
+        <v>-0.003431574896010492</v>
       </c>
       <c r="C59" t="n">
-        <v>3.160610218006956</v>
+        <v>2.698924329140925</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4533470658120883</v>
+        <v>0.4359465034741501</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0002266735329060441</v>
+        <v>0.000217973251737075</v>
       </c>
     </row>
     <row r="60">
@@ -1609,16 +1609,16 @@
         <v>44165</v>
       </c>
       <c r="B60" t="n">
-        <v>0.07763625597150196</v>
+        <v>0.07479490367978577</v>
       </c>
       <c r="C60" t="n">
-        <v>3.405988161918289</v>
+        <v>2.90079011437805</v>
       </c>
       <c r="D60" t="n">
-        <v>0.3161697129318637</v>
+        <v>0.3181093866281378</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0001580848564659319</v>
+        <v>0.0001590546933140689</v>
       </c>
     </row>
     <row r="61">
@@ -1626,16 +1626,16 @@
         <v>44196</v>
       </c>
       <c r="B61" t="n">
-        <v>0.02790895849773529</v>
+        <v>0.0246084692543231</v>
       </c>
       <c r="C61" t="n">
-        <v>3.501045744173044</v>
+        <v>2.972174118720967</v>
       </c>
       <c r="D61" t="n">
-        <v>0.4182420190535986</v>
+        <v>0.4855511198581151</v>
       </c>
       <c r="E61" t="n">
-        <v>0.0002091210095267993</v>
+        <v>0.0002427755599290576</v>
       </c>
     </row>
     <row r="62">
@@ -1643,16 +1643,16 @@
         <v>44225</v>
       </c>
       <c r="B62" t="n">
-        <v>0.009411542046647455</v>
+        <v>0.005401762569742024</v>
       </c>
       <c r="C62" t="n">
-        <v>3.533995983401564</v>
+        <v>2.98822909762623</v>
       </c>
       <c r="D62" t="n">
-        <v>0.3245994709955092</v>
+        <v>0.3934136265860301</v>
       </c>
       <c r="E62" t="n">
-        <v>0.0001622997354977546</v>
+        <v>0.000196706813293015</v>
       </c>
     </row>
     <row r="63">
@@ -1660,16 +1660,16 @@
         <v>44253</v>
       </c>
       <c r="B63" t="n">
-        <v>0.1234004332312319</v>
+        <v>0.1081276389348744</v>
       </c>
       <c r="C63" t="n">
-        <v>3.970092618790751</v>
+        <v>3.311339254549044</v>
       </c>
       <c r="D63" t="n">
-        <v>0.3814330802596496</v>
+        <v>0.465004338066764</v>
       </c>
       <c r="E63" t="n">
-        <v>0.0001907165401298248</v>
+        <v>0.000232502169033382</v>
       </c>
     </row>
     <row r="64">
@@ -1677,16 +1677,16 @@
         <v>44286</v>
       </c>
       <c r="B64" t="n">
-        <v>0.06094657068683591</v>
+        <v>0.0568196467056849</v>
       </c>
       <c r="C64" t="n">
-        <v>4.212056149215167</v>
+        <v>3.499488381115187</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4125340209780601</v>
+        <v>0.4358920235533172</v>
       </c>
       <c r="E64" t="n">
-        <v>0.0002062670104890301</v>
+        <v>0.0002179460117766586</v>
       </c>
     </row>
     <row r="65">
@@ -1694,16 +1694,16 @@
         <v>44316</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0541432463807851</v>
+        <v>0.04852106117678381</v>
       </c>
       <c r="C65" t="n">
-        <v>4.440110543071825</v>
+        <v>3.669287270942722</v>
       </c>
       <c r="D65" t="n">
-        <v>0.278207983566949</v>
+        <v>0.2906539287560582</v>
       </c>
       <c r="E65" t="n">
-        <v>0.0001391039917834745</v>
+        <v>0.0001453269643780291</v>
       </c>
     </row>
     <row r="66">
@@ -1711,16 +1711,16 @@
         <v>44344</v>
       </c>
       <c r="B66" t="n">
-        <v>0.03494281406331538</v>
+        <v>0.03454565395840726</v>
       </c>
       <c r="C66" t="n">
-        <v>4.59526050019895</v>
+        <v>3.796045199278697</v>
       </c>
       <c r="D66" t="n">
-        <v>0.3428250744876514</v>
+        <v>0.4128859135970886</v>
       </c>
       <c r="E66" t="n">
-        <v>0.0001714125372438257</v>
+        <v>0.0002064429567985443</v>
       </c>
     </row>
     <row r="67">
@@ -1728,16 +1728,16 @@
         <v>44377</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.02095468974639128</v>
+        <v>-0.01632109998473817</v>
       </c>
       <c r="C67" t="n">
-        <v>4.498968242113435</v>
+        <v>3.734089566034684</v>
       </c>
       <c r="D67" t="n">
-        <v>0.3109046548336711</v>
+        <v>0.3852710109205802</v>
       </c>
       <c r="E67" t="n">
-        <v>0.0001554523274168355</v>
+        <v>0.0001926355054602901</v>
       </c>
     </row>
     <row r="68">
@@ -1745,16 +1745,16 @@
         <v>44407</v>
       </c>
       <c r="B68" t="n">
-        <v>0.01169684987726245</v>
+        <v>0.01919420638049786</v>
       </c>
       <c r="C68" t="n">
-        <v>4.551591998244007</v>
+        <v>3.805762451808418</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2669782281765481</v>
+        <v>0.2880704424048206</v>
       </c>
       <c r="E68" t="n">
-        <v>0.000133489114088274</v>
+        <v>0.0001440352212024103</v>
       </c>
     </row>
     <row r="69">
@@ -1762,16 +1762,16 @@
         <v>44439</v>
       </c>
       <c r="B69" t="n">
-        <v>0.06266493018817157</v>
+        <v>0.05499821947353092</v>
       </c>
       <c r="C69" t="n">
-        <v>4.836817193059008</v>
+        <v>4.015072610397101</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5926754031766892</v>
+        <v>0.5914628928954176</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0002963377015883446</v>
+        <v>0.0002957314464477088</v>
       </c>
     </row>
     <row r="70">
@@ -1779,16 +1779,16 @@
         <v>44469</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.0570809060417004</v>
+        <v>-0.05985855643522537</v>
       </c>
       <c r="C70" t="n">
-        <v>4.560727285321126</v>
+        <v>3.774736159956118</v>
       </c>
       <c r="D70" t="n">
-        <v>0.4042001473902915</v>
+        <v>0.32440173884359</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0002021000736951457</v>
+        <v>0.000162200869421795</v>
       </c>
     </row>
     <row r="71">
@@ -1796,16 +1796,16 @@
         <v>44498</v>
       </c>
       <c r="B71" t="n">
-        <v>0.07422778816448246</v>
+        <v>0.07300249296911165</v>
       </c>
       <c r="C71" t="n">
-        <v>4.899259984131917</v>
+        <v>4.050301309933565</v>
       </c>
       <c r="D71" t="n">
-        <v>0.5077034791260056</v>
+        <v>0.4825261426171357</v>
       </c>
       <c r="E71" t="n">
-        <v>0.0002538517395630028</v>
+        <v>0.0002412630713085679</v>
       </c>
     </row>
     <row r="72">
@@ -1813,16 +1813,16 @@
         <v>44530</v>
       </c>
       <c r="B72" t="n">
-        <v>0.02707484729318137</v>
+        <v>0.01520780030976114</v>
       </c>
       <c r="C72" t="n">
-        <v>5.031906700051883</v>
+        <v>4.111897483449399</v>
       </c>
       <c r="D72" t="n">
-        <v>0.4648981066350413</v>
+        <v>0.4261198201517571</v>
       </c>
       <c r="E72" t="n">
-        <v>0.0002324490533175206</v>
+        <v>0.0002130599100758785</v>
       </c>
     </row>
     <row r="73">
@@ -1830,16 +1830,16 @@
         <v>44561</v>
       </c>
       <c r="B73" t="n">
-        <v>0.05876567740443597</v>
+        <v>0.03810200022130483</v>
       </c>
       <c r="C73" t="n">
-        <v>5.327610105916353</v>
+        <v>4.268569002273771</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5247656127956974</v>
+        <v>0.5196450657330702</v>
       </c>
       <c r="E73" t="n">
-        <v>0.0002623828063978487</v>
+        <v>0.0002598225328665351</v>
       </c>
     </row>
     <row r="74">
@@ -1847,16 +1847,16 @@
         <v>44592</v>
       </c>
       <c r="B74" t="n">
-        <v>-0.0749306427198332</v>
+        <v>-0.0604158581664304</v>
       </c>
       <c r="C74" t="n">
-        <v>4.928408856519362</v>
+        <v>4.010679742858778</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5488329217667848</v>
+        <v>0.6469799721116429</v>
       </c>
       <c r="E74" t="n">
-        <v>0.0002744164608833924</v>
+        <v>0.0003234899860558215</v>
       </c>
     </row>
     <row r="75">
@@ -1864,16 +1864,16 @@
         <v>44620</v>
       </c>
       <c r="B75" t="n">
-        <v>0.0133763822776881</v>
+        <v>0.0105654196959086</v>
       </c>
       <c r="C75" t="n">
-        <v>4.994333137404908</v>
+        <v>4.053054257607959</v>
       </c>
       <c r="D75" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.611111111111111</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0003333333333333333</v>
+        <v>0.0003055555555555555</v>
       </c>
     </row>
     <row r="76">
@@ -1881,16 +1881,16 @@
         <v>44651</v>
       </c>
       <c r="B76" t="n">
-        <v>0.04855296873254384</v>
+        <v>0.03190431332762872</v>
       </c>
       <c r="C76" t="n">
-        <v>5.236822838065236</v>
+        <v>4.182364170576563</v>
       </c>
       <c r="D76" t="n">
-        <v>0.4157169490742614</v>
+        <v>0.4279744554900177</v>
       </c>
       <c r="E76" t="n">
-        <v>0.0002078584745371307</v>
+        <v>0.0002139872277450088</v>
       </c>
     </row>
     <row r="77">
@@ -1898,16 +1898,16 @@
         <v>44680</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.01838669528103145</v>
+        <v>-0.02609524743262456</v>
       </c>
       <c r="C77" t="n">
-        <v>5.140534972300984</v>
+        <v>4.073224342692024</v>
       </c>
       <c r="D77" t="n">
-        <v>0.4793549876889186</v>
+        <v>0.5872423368164741</v>
       </c>
       <c r="E77" t="n">
-        <v>0.0002396774938444593</v>
+        <v>0.000293621168408237</v>
       </c>
     </row>
     <row r="78">
@@ -1915,16 +1915,16 @@
         <v>44712</v>
       </c>
       <c r="B78" t="n">
-        <v>0.009158663096936021</v>
+        <v>0.009000710159863647</v>
       </c>
       <c r="C78" t="n">
-        <v>5.187615400250307</v>
+        <v>4.109886254416696</v>
       </c>
       <c r="D78" t="n">
-        <v>0.3348652382633098</v>
+        <v>0.3580706861802599</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0001674326191316549</v>
+        <v>0.00017903534309013</v>
       </c>
     </row>
     <row r="79">
@@ -1932,16 +1932,16 @@
         <v>44742</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.04676474155740319</v>
+        <v>-0.04354163727255976</v>
       </c>
       <c r="C79" t="n">
-        <v>4.945017906758396</v>
+        <v>3.930935077895405</v>
       </c>
       <c r="D79" t="n">
-        <v>0.390688007925762</v>
+        <v>0.4307499712910187</v>
       </c>
       <c r="E79" t="n">
-        <v>0.000195344003962881</v>
+        <v>0.0002153749856455093</v>
       </c>
     </row>
     <row r="80">
@@ -1949,16 +1949,16 @@
         <v>44771</v>
       </c>
       <c r="B80" t="n">
-        <v>0.02279417510983917</v>
+        <v>0.02245975323193681</v>
       </c>
       <c r="C80" t="n">
-        <v>5.057735510846338</v>
+        <v>4.0192229097157</v>
       </c>
       <c r="D80" t="n">
-        <v>0.4954540594625106</v>
+        <v>0.4598025948070907</v>
       </c>
       <c r="E80" t="n">
-        <v>0.0002477270297312553</v>
+        <v>0.0002299012974035453</v>
       </c>
     </row>
     <row r="81">
@@ -1966,16 +1966,16 @@
         <v>44804</v>
       </c>
       <c r="B81" t="n">
-        <v>0.007476783142942444</v>
+        <v>0.003392455010138115</v>
       </c>
       <c r="C81" t="n">
-        <v>5.095551102455295</v>
+        <v>4.032857942612627</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.35</v>
       </c>
       <c r="E81" t="n">
-        <v>0.0001666666666666667</v>
+        <v>0.000175</v>
       </c>
     </row>
     <row r="82">
@@ -1983,16 +1983,16 @@
         <v>44834</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.03654895421124371</v>
+        <v>-0.03661450013995093</v>
       </c>
       <c r="C82" t="n">
-        <v>4.909314038530605</v>
+        <v>3.885196864908435</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3556020863822599</v>
+        <v>0.433002789276732</v>
       </c>
       <c r="E82" t="n">
-        <v>0.00017780104319113</v>
+        <v>0.000216501394638366</v>
       </c>
     </row>
     <row r="83">
@@ -2000,16 +2000,16 @@
         <v>44865</v>
       </c>
       <c r="B83" t="n">
-        <v>0.09027511606292449</v>
+        <v>0.0819183876110267</v>
       </c>
       <c r="C83" t="n">
-        <v>5.352502933148299</v>
+        <v>4.20346592763315</v>
       </c>
       <c r="D83" t="n">
-        <v>0.389808285371838</v>
+        <v>0.407386921851623</v>
       </c>
       <c r="E83" t="n">
-        <v>0.000194904142685919</v>
+        <v>0.0002036934609258115</v>
       </c>
     </row>
     <row r="84">
@@ -2017,16 +2017,16 @@
         <v>44895</v>
       </c>
       <c r="B84" t="n">
-        <v>0.03271636993490246</v>
+        <v>0.02967831467536709</v>
       </c>
       <c r="C84" t="n">
-        <v>5.52761739918683</v>
+        <v>4.328217712160631</v>
       </c>
       <c r="D84" t="n">
-        <v>0.4197450394005079</v>
+        <v>0.3813014360752536</v>
       </c>
       <c r="E84" t="n">
-        <v>0.000209872519700254</v>
+        <v>0.0001906507180376268</v>
       </c>
     </row>
     <row r="85">
@@ -2034,16 +2034,16 @@
         <v>44925</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.02300580126546433</v>
+        <v>-0.02202370422493135</v>
       </c>
       <c r="C85" t="n">
-        <v>5.400450131829614</v>
+        <v>4.232894325446896</v>
       </c>
       <c r="D85" t="n">
-        <v>0.4417176809527585</v>
+        <v>0.5162260002031496</v>
       </c>
       <c r="E85" t="n">
-        <v>0.0002208588404763792</v>
+        <v>0.0002581130001015748</v>
       </c>
     </row>
     <row r="86">
@@ -2051,16 +2051,16 @@
         <v>44957</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.008199735220295372</v>
+        <v>-0.003234623779887757</v>
       </c>
       <c r="C86" t="n">
-        <v>5.356167870678202</v>
+        <v>4.219202504804054</v>
       </c>
       <c r="D86" t="n">
-        <v>0.281248910888328</v>
+        <v>0.2798589530848426</v>
       </c>
       <c r="E86" t="n">
-        <v>0.000140624455444164</v>
+        <v>0.0001399294765424213</v>
       </c>
     </row>
     <row r="87">
@@ -2068,16 +2068,16 @@
         <v>44985</v>
       </c>
       <c r="B87" t="n">
-        <v>-0.04123695768674585</v>
+        <v>-0.03390802680468675</v>
       </c>
       <c r="C87" t="n">
-        <v>5.135295802831937</v>
+        <v>4.076137673176756</v>
       </c>
       <c r="D87" t="n">
-        <v>0.6671491323561385</v>
+        <v>0.5988524062714413</v>
       </c>
       <c r="E87" t="n">
-        <v>0.0003335745661780693</v>
+        <v>0.0002994262031357206</v>
       </c>
     </row>
     <row r="88">
@@ -2085,16 +2085,16 @@
         <v>45016</v>
       </c>
       <c r="B88" t="n">
-        <v>0.01940297459504217</v>
+        <v>0.01548292718019174</v>
       </c>
       <c r="C88" t="n">
-        <v>5.234935816832312</v>
+        <v>4.139248215946989</v>
       </c>
       <c r="D88" t="n">
-        <v>0.7427698798145271</v>
+        <v>0.7773842477535232</v>
       </c>
       <c r="E88" t="n">
-        <v>0.0003713849399072636</v>
+        <v>0.0003886921238767616</v>
       </c>
     </row>
     <row r="89">
@@ -2102,16 +2102,16 @@
         <v>45044</v>
       </c>
       <c r="B89" t="n">
-        <v>0.01654413490706072</v>
+        <v>0.01587336034740303</v>
       </c>
       <c r="C89" t="n">
-        <v>5.32154330121579</v>
+        <v>4.20495199444606</v>
       </c>
       <c r="D89" t="n">
-        <v>0.4546602648051472</v>
+        <v>0.3827026271973891</v>
       </c>
       <c r="E89" t="n">
-        <v>0.0002273301324025736</v>
+        <v>0.0001913513135986946</v>
       </c>
     </row>
     <row r="90">
@@ -2119,16 +2119,16 @@
         <v>45077</v>
       </c>
       <c r="B90" t="n">
-        <v>0.008370427348336696</v>
+        <v>0.00674156473299588</v>
       </c>
       <c r="C90" t="n">
-        <v>5.366086892799645</v>
+        <v>4.233299950515758</v>
       </c>
       <c r="D90" t="n">
-        <v>0.5522757043527035</v>
+        <v>0.5426380880056079</v>
       </c>
       <c r="E90" t="n">
-        <v>0.0002761378521763518</v>
+        <v>0.000271319044002804</v>
       </c>
     </row>
     <row r="91">
@@ -2136,16 +2136,16 @@
         <v>45107</v>
       </c>
       <c r="B91" t="n">
-        <v>0.07906422481609285</v>
+        <v>0.07421989751904784</v>
       </c>
       <c r="C91" t="n">
-        <v>5.790352393274645</v>
+        <v>4.547495039010428</v>
       </c>
       <c r="D91" t="n">
-        <v>0.7337052482147789</v>
+        <v>0.5254605492210932</v>
       </c>
       <c r="E91" t="n">
-        <v>0.0003668526241073894</v>
+        <v>0.0002627302746105466</v>
       </c>
     </row>
     <row r="92">
@@ -2153,16 +2153,16 @@
         <v>45138</v>
       </c>
       <c r="B92" t="n">
-        <v>0.0323838155918706</v>
+        <v>0.02821800209103426</v>
       </c>
       <c r="C92" t="n">
-        <v>5.977866097390398</v>
+        <v>4.675816263530193</v>
       </c>
       <c r="D92" t="n">
-        <v>0.3972141996720182</v>
+        <v>0.3047302186014228</v>
       </c>
       <c r="E92" t="n">
-        <v>0.0001986070998360091</v>
+        <v>0.0001523651093007114</v>
       </c>
     </row>
     <row r="93">
@@ -2170,16 +2170,16 @@
         <v>45169</v>
       </c>
       <c r="B93" t="n">
-        <v>-0.01001314967263404</v>
+        <v>-0.005346808936551991</v>
       </c>
       <c r="C93" t="n">
-        <v>5.918008829434263</v>
+        <v>4.650815567346674</v>
       </c>
       <c r="D93" t="n">
-        <v>0.4769606446792568</v>
+        <v>0.3591593636929031</v>
       </c>
       <c r="E93" t="n">
-        <v>0.0002384803223396284</v>
+        <v>0.0001795796818464516</v>
       </c>
     </row>
     <row r="94">
@@ -2187,16 +2187,16 @@
         <v>45198</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.05450807420350591</v>
+        <v>-0.04774382822617028</v>
       </c>
       <c r="C94" t="n">
-        <v>5.595429565022457</v>
+        <v>4.428767827787676</v>
       </c>
       <c r="D94" t="n">
-        <v>0.4461129716743044</v>
+        <v>0.4636835516474806</v>
       </c>
       <c r="E94" t="n">
-        <v>0.0002230564858371522</v>
+        <v>0.0002318417758237403</v>
       </c>
     </row>
     <row r="95">
@@ -2204,16 +2204,16 @@
         <v>45230</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.009510658798504164</v>
+        <v>-0.003887570454753917</v>
       </c>
       <c r="C95" t="n">
-        <v>5.542213343598466</v>
+        <v>4.411550680829404</v>
       </c>
       <c r="D95" t="n">
-        <v>0.5234120666257756</v>
+        <v>0.4176859842713856</v>
       </c>
       <c r="E95" t="n">
-        <v>0.0002617060333128878</v>
+        <v>0.0002088429921356928</v>
       </c>
     </row>
     <row r="96">
@@ -2221,16 +2221,16 @@
         <v>45260</v>
       </c>
       <c r="B96" t="n">
-        <v>0.07681147470534268</v>
+        <v>0.08354223761188978</v>
       </c>
       <c r="C96" t="n">
-        <v>5.967918923651893</v>
+        <v>4.780101496044147</v>
       </c>
       <c r="D96" t="n">
-        <v>0.6864507360493926</v>
+        <v>0.5087629800701975</v>
       </c>
       <c r="E96" t="n">
-        <v>0.0003432253680246963</v>
+        <v>0.0002543814900350987</v>
       </c>
     </row>
     <row r="97">
@@ -2238,16 +2238,16 @@
         <v>45289</v>
       </c>
       <c r="B97" t="n">
-        <v>0.03678182225220168</v>
+        <v>0.02779357121580579</v>
       </c>
       <c r="C97" t="n">
-        <v>6.187429856717207</v>
+        <v>4.91295758739323</v>
       </c>
       <c r="D97" t="n">
-        <v>0.5790910557213309</v>
+        <v>0.487171932444869</v>
       </c>
       <c r="E97" t="n">
-        <v>0.0002895455278606654</v>
+        <v>0.0002435859662224345</v>
       </c>
     </row>
     <row r="98">
@@ -2255,16 +2255,16 @@
         <v>45322</v>
       </c>
       <c r="B98" t="n">
-        <v>0.05174227210247903</v>
+        <v>0.04105046741517471</v>
       </c>
       <c r="C98" t="n">
-        <v>6.507581535978471</v>
+        <v>5.114636792746651</v>
       </c>
       <c r="D98" t="n">
-        <v>0.6069081236493726</v>
+        <v>0.6089022962485331</v>
       </c>
       <c r="E98" t="n">
-        <v>0.0003034540618246863</v>
+        <v>0.0003044511481242665</v>
       </c>
     </row>
     <row r="99">
@@ -2272,16 +2272,16 @@
         <v>45351</v>
       </c>
       <c r="B99" t="n">
-        <v>0.1043774862716613</v>
+        <v>0.07835372666623351</v>
       </c>
       <c r="C99" t="n">
-        <v>7.186826538411781</v>
+        <v>5.515387646002583</v>
       </c>
       <c r="D99" t="n">
-        <v>0.443821719445891</v>
+        <v>0.566575433849842</v>
       </c>
       <c r="E99" t="n">
-        <v>0.0002219108597229455</v>
+        <v>0.000283287716924921</v>
       </c>
     </row>
     <row r="100">
@@ -2289,16 +2289,16 @@
         <v>45379</v>
       </c>
       <c r="B100" t="n">
-        <v>0.04835086144890611</v>
+        <v>0.0504887889905963</v>
       </c>
       <c r="C100" t="n">
-        <v>7.53431579262785</v>
+        <v>5.79385288906295</v>
       </c>
       <c r="D100" t="n">
-        <v>0.5451967507432014</v>
+        <v>0.483804888593411</v>
       </c>
       <c r="E100" t="n">
-        <v>0.0002725983753716007</v>
+        <v>0.0002419024442967055</v>
       </c>
     </row>
     <row r="101">
@@ -2306,16 +2306,16 @@
         <v>45412</v>
       </c>
       <c r="B101" t="n">
-        <v>0.01376624502499927</v>
+        <v>0.01161687740110535</v>
       </c>
       <c r="C101" t="n">
-        <v>7.638035029924887</v>
+        <v>5.861159367755234</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5236812382109461</v>
+        <v>0.4867391990275767</v>
       </c>
       <c r="E101" t="n">
-        <v>0.0002618406191054731</v>
+        <v>0.0002433695995137883</v>
       </c>
     </row>
     <row r="102">
@@ -2323,16 +2323,16 @@
         <v>45443</v>
       </c>
       <c r="B102" t="n">
-        <v>0.0518223128192413</v>
+        <v>0.04734465698781701</v>
       </c>
       <c r="C102" t="n">
-        <v>8.033855670569977</v>
+        <v>6.138653947572537</v>
       </c>
       <c r="D102" t="n">
-        <v>0.2813294588030321</v>
+        <v>0.2121208518792058</v>
       </c>
       <c r="E102" t="n">
-        <v>0.000140664729401516</v>
+        <v>0.0001060604259396029</v>
       </c>
     </row>
     <row r="103">
@@ -2340,16 +2340,16 @@
         <v>45471</v>
       </c>
       <c r="B103" t="n">
-        <v>0.007234510852013602</v>
+        <v>0.005512164274004353</v>
       </c>
       <c r="C103" t="n">
-        <v>8.091976686602226</v>
+        <v>6.172491216552822</v>
       </c>
       <c r="D103" t="n">
-        <v>0.2031767730068406</v>
+        <v>0.2913435961713294</v>
       </c>
       <c r="E103" t="n">
-        <v>0.0001015883865034203</v>
+        <v>0.0001456717980856647</v>
       </c>
     </row>
     <row r="104">
@@ -2357,16 +2357,16 @@
         <v>45504</v>
       </c>
       <c r="B104" t="n">
-        <v>-0.02098174944549825</v>
+        <v>-0.02372994770635549</v>
       </c>
       <c r="C104" t="n">
-        <v>7.922192859245126</v>
+        <v>6.026018322766085</v>
       </c>
       <c r="D104" t="n">
-        <v>0.4358533248303565</v>
+        <v>0.4398721471674549</v>
       </c>
       <c r="E104" t="n">
-        <v>0.0002179266624151783</v>
+        <v>0.0002199360735837274</v>
       </c>
     </row>
     <row r="105">
@@ -2374,16 +2374,16 @@
         <v>45534</v>
       </c>
       <c r="B105" t="n">
-        <v>0.03562787735235895</v>
+        <v>0.03412098212741433</v>
       </c>
       <c r="C105" t="n">
-        <v>8.204443774796045</v>
+        <v>6.231631986256658</v>
       </c>
       <c r="D105" t="n">
-        <v>0.512650876731762</v>
+        <v>0.5647512983235172</v>
       </c>
       <c r="E105" t="n">
-        <v>0.000256325438365881</v>
+        <v>0.0002823756491617586</v>
       </c>
     </row>
     <row r="106">
@@ -2391,16 +2391,16 @@
         <v>45565</v>
       </c>
       <c r="B106" t="n">
-        <v>0.03532627968923181</v>
+        <v>0.02888846871682908</v>
       </c>
       <c r="C106" t="n">
-        <v>8.494276250279066</v>
+        <v>6.411654291946425</v>
       </c>
       <c r="D106" t="n">
-        <v>0.4287796200828571</v>
+        <v>0.5374397286144004</v>
       </c>
       <c r="E106" t="n">
-        <v>0.0002143898100414286</v>
+        <v>0.0002687198643072002</v>
       </c>
     </row>
     <row r="107">
@@ -2408,16 +2408,16 @@
         <v>45596</v>
       </c>
       <c r="B107" t="n">
-        <v>0.008966105346823692</v>
+        <v>0.005141311578049429</v>
       </c>
       <c r="C107" t="n">
-        <v>8.570436825984091</v>
+        <v>6.444618604392059</v>
       </c>
       <c r="D107" t="n">
-        <v>0.4708253481479272</v>
+        <v>0.4180738222831388</v>
       </c>
       <c r="E107" t="n">
-        <v>0.0002354126740739636</v>
+        <v>0.0002090369111415694</v>
       </c>
     </row>
     <row r="108">
@@ -2425,16 +2425,16 @@
         <v>45625</v>
       </c>
       <c r="B108" t="n">
-        <v>0.06484512667623665</v>
+        <v>0.0748230230497459</v>
       </c>
       <c r="C108" t="n">
-        <v>9.126187887635712</v>
+        <v>6.926824450775308</v>
       </c>
       <c r="D108" t="n">
-        <v>0.4</v>
+        <v>0.4760574753327102</v>
       </c>
       <c r="E108" t="n">
-        <v>0.0002</v>
+        <v>0.0002380287376663551</v>
       </c>
     </row>
     <row r="109">
@@ -2442,16 +2442,16 @@
         <v>45657</v>
       </c>
       <c r="B109" t="n">
-        <v>-0.04365116344344652</v>
+        <v>-0.04213909759741569</v>
       </c>
       <c r="C109" t="n">
-        <v>8.727819168536923</v>
+        <v>6.634934319203922</v>
       </c>
       <c r="D109" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.4077855295842431</v>
       </c>
       <c r="E109" t="n">
-        <v>0.0002333333333333334</v>
+        <v>0.0002038927647921215</v>
       </c>
     </row>
     <row r="110">
@@ -2459,16 +2459,16 @@
         <v>45688</v>
       </c>
       <c r="B110" t="n">
-        <v>0.04632848675558485</v>
+        <v>0.05004961796471612</v>
       </c>
       <c r="C110" t="n">
-        <v>9.132165823291626</v>
+        <v>6.967010247101062</v>
       </c>
       <c r="D110" t="n">
-        <v>0.5368887265125979</v>
+        <v>0.5093100188986167</v>
       </c>
       <c r="E110" t="n">
-        <v>0.000268444363256299</v>
+        <v>0.0002546550094493084</v>
       </c>
     </row>
     <row r="111">
@@ -2476,16 +2476,16 @@
         <v>45716</v>
       </c>
       <c r="B111" t="n">
-        <v>-0.004944614825351079</v>
+        <v>-0.004510385539992146</v>
       </c>
       <c r="C111" t="n">
-        <v>9.087010780774213</v>
+        <v>6.935586344825561</v>
       </c>
       <c r="D111" t="n">
-        <v>0.5402372244037155</v>
+        <v>0.5722373151874032</v>
       </c>
       <c r="E111" t="n">
-        <v>0.0002701186122018577</v>
+        <v>0.0002861186575937016</v>
       </c>
     </row>
     <row r="112">
@@ -2493,16 +2493,16 @@
         <v>45747</v>
       </c>
       <c r="B112" t="n">
-        <v>-0.02154750831535711</v>
+        <v>-0.02414206548884844</v>
       </c>
       <c r="C112" t="n">
-        <v>8.891208340413741</v>
+        <v>6.768146965085219</v>
       </c>
       <c r="D112" t="n">
-        <v>0.7396923362936948</v>
+        <v>0.6328711899762145</v>
       </c>
       <c r="E112" t="n">
-        <v>0.0003698461681468474</v>
+        <v>0.0003164355949881072</v>
       </c>
     </row>
     <row r="113">
@@ -2510,16 +2510,16 @@
         <v>45777</v>
       </c>
       <c r="B113" t="n">
-        <v>0.002882647731849416</v>
+        <v>0.006914538235799295</v>
       </c>
       <c r="C113" t="n">
-        <v>8.916838561969634</v>
+        <v>6.81494557606081</v>
       </c>
       <c r="D113" t="n">
-        <v>0.5110245795530017</v>
+        <v>0.4995218927360559</v>
       </c>
       <c r="E113" t="n">
-        <v>0.0002555122897765009</v>
+        <v>0.0002497609463680279</v>
       </c>
     </row>
     <row r="114">
@@ -2527,16 +2527,16 @@
         <v>45807</v>
       </c>
       <c r="B114" t="n">
-        <v>0.006704298393372125</v>
+        <v>0.0202486411276458</v>
       </c>
       <c r="C114" t="n">
-        <v>8.976619708414605</v>
+        <v>6.952938963334903</v>
       </c>
       <c r="D114" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.2999999999999999</v>
       </c>
       <c r="E114" t="n">
-        <v>0.0002</v>
+        <v>0.00015</v>
       </c>
     </row>
     <row r="115">
@@ -2544,16 +2544,16 @@
         <v>45838</v>
       </c>
       <c r="B115" t="n">
-        <v>0.05093283976768379</v>
+        <v>0.04821044245593503</v>
       </c>
       <c r="C115" t="n">
-        <v>9.433824441678718</v>
+        <v>7.28814322712639</v>
       </c>
       <c r="D115" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.4764598240043006</v>
       </c>
       <c r="E115" t="n">
-        <v>0.0003</v>
+        <v>0.0002382299120021503</v>
       </c>
     </row>
     <row r="116">
@@ -2561,16 +2561,16 @@
         <v>45869</v>
       </c>
       <c r="B116" t="n">
-        <v>0.01138647003040751</v>
+        <v>0.01403383387077748</v>
       </c>
       <c r="C116" t="n">
-        <v>9.541242400956019</v>
+        <v>7.390423818402313</v>
       </c>
       <c r="D116" t="n">
-        <v>0.4863911536556649</v>
+        <v>0.4557814001106011</v>
       </c>
       <c r="E116" t="n">
-        <v>0.0002431955768278325</v>
+        <v>0.0002278907000553006</v>
       </c>
     </row>
     <row r="117">
@@ -2578,16 +2578,16 @@
         <v>45898</v>
       </c>
       <c r="B117" t="n">
-        <v>0.006442972198887978</v>
+        <v>0.006697826779785631</v>
       </c>
       <c r="C117" t="n">
-        <v>9.602716360488229</v>
+        <v>7.439923596967175</v>
       </c>
       <c r="D117" t="n">
-        <v>0.5411893729471376</v>
+        <v>0.5226098720929405</v>
       </c>
       <c r="E117" t="n">
-        <v>0.0002705946864735688</v>
+        <v>0.0002613049360464703</v>
       </c>
     </row>
     <row r="118">
@@ -2595,16 +2595,16 @@
         <v>45930</v>
       </c>
       <c r="B118" t="n">
-        <v>0.09731575328714215</v>
+        <v>0.07756293665020352</v>
       </c>
       <c r="C118" t="n">
-        <v>10.5372119367119</v>
+        <v>8.016985919601094</v>
       </c>
       <c r="D118" t="n">
-        <v>0.3922827997295384</v>
+        <v>0.2942413915272979</v>
       </c>
       <c r="E118" t="n">
-        <v>0.0001961413998647692</v>
+        <v>0.0001471206957636489</v>
       </c>
     </row>
     <row r="119">
@@ -2612,16 +2612,16 @@
         <v>45961</v>
       </c>
       <c r="B119" t="n">
-        <v>0.07700324272910913</v>
+        <v>0.06647206952604656</v>
       </c>
       <c r="C119" t="n">
-        <v>11.3486114251626</v>
+        <v>8.549891565038154</v>
       </c>
       <c r="D119" t="n">
-        <v>0.4668886004511975</v>
+        <v>0.5067228172861363</v>
       </c>
       <c r="E119" t="n">
-        <v>0.0002334443002255987</v>
+        <v>0.0002533614086430682</v>
       </c>
     </row>
     <row r="120">
@@ -2629,16 +2629,16 @@
         <v>45989</v>
       </c>
       <c r="B120" t="n">
-        <v>0.05931685326130086</v>
+        <v>0.04641178960643928</v>
       </c>
       <c r="C120" t="n">
-        <v>12.02177534378849</v>
+        <v>8.946707333512574</v>
       </c>
       <c r="D120" t="n">
-        <v>0.3413730148814737</v>
+        <v>0.3489416401360022</v>
       </c>
       <c r="E120" t="n">
-        <v>0.0001706865074407369</v>
+        <v>0.0001744708200680011</v>
       </c>
     </row>
     <row r="121">
@@ -2646,16 +2646,16 @@
         <v>46022</v>
       </c>
       <c r="B121" t="n">
-        <v>0.04185152065198344</v>
+        <v>0.01170977376460987</v>
       </c>
       <c r="C121" t="n">
-        <v>12.52490492286256</v>
+        <v>9.051471252326182</v>
       </c>
       <c r="D121" t="n">
-        <v>0.2200736256351608</v>
+        <v>0.3143812872731168</v>
       </c>
       <c r="E121" t="n">
-        <v>0.0001100368128175804</v>
+        <v>0.0001571906436365584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>